<commit_message>
intend and path restored
</commit_message>
<xml_diff>
--- a/output/roundtrip.xlsx
+++ b/output/roundtrip.xlsx
@@ -774,12 +774,12 @@
       <c r="AD3" t="inlineStr"/>
       <c r="AE3" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF3" t="inlineStr">
         <is>
-          <t>@version</t>
+          <t>processDataSet/@version</t>
         </is>
       </c>
     </row>
@@ -864,12 +864,12 @@
       <c r="AD4" t="inlineStr"/>
       <c r="AE4" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF4" t="inlineStr">
         <is>
-          <t>@epd2:epd-version</t>
+          <t>processDataSet/@epd2:epd-version</t>
         </is>
       </c>
     </row>
@@ -962,12 +962,12 @@
       <c r="AD5" t="inlineStr"/>
       <c r="AE5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AF5" t="inlineStr">
         <is>
-          <t>@locations</t>
+          <t>processDataSet/@locations</t>
         </is>
       </c>
     </row>
@@ -1060,12 +1060,12 @@
       <c r="AD6" t="inlineStr"/>
       <c r="AE6" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF6" t="inlineStr">
         <is>
-          <t>@metaDataOnly</t>
+          <t>processDataSet/@locations/@metaDataOnly</t>
         </is>
       </c>
     </row>
@@ -1248,12 +1248,12 @@
       <c r="AD8" t="inlineStr"/>
       <c r="AE8" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AF8" t="inlineStr">
         <is>
-          <t>dataSetInformation</t>
+          <t>processInformation/dataSetInformation</t>
         </is>
       </c>
     </row>
@@ -1358,12 +1358,12 @@
       <c r="AD9" t="inlineStr"/>
       <c r="AE9" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF9" t="inlineStr">
         <is>
-          <t>UUID</t>
+          <t>processInformation/dataSetInformation/UUID</t>
         </is>
       </c>
     </row>
@@ -1476,12 +1476,12 @@
       <c r="AD10" t="inlineStr"/>
       <c r="AE10" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF10" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>processInformation/dataSetInformation/name</t>
         </is>
       </c>
     </row>
@@ -1582,12 +1582,12 @@
       <c r="AD11" t="inlineStr"/>
       <c r="AE11" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF11" t="inlineStr">
         <is>
-          <t>baseName</t>
+          <t>processInformation/dataSetInformation/baseName</t>
         </is>
       </c>
     </row>
@@ -1688,12 +1688,12 @@
       <c r="AD12" t="inlineStr"/>
       <c r="AE12" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF12" t="inlineStr">
         <is>
-          <t>functionalUnitFlowProperties</t>
+          <t>processInformation/dataSetInformation/functionalUnitFlowProperties</t>
         </is>
       </c>
     </row>
@@ -1782,12 +1782,12 @@
       <c r="AD13" t="inlineStr"/>
       <c r="AE13" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF13" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>processInformation/dataSetInformation/other</t>
         </is>
       </c>
     </row>
@@ -1884,12 +1884,12 @@
       <c r="AD14" t="inlineStr"/>
       <c r="AE14" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF14" t="inlineStr">
         <is>
-          <t>synonyms</t>
+          <t>processInformation/dataSetInformation/synonyms</t>
         </is>
       </c>
     </row>
@@ -1993,12 +1993,12 @@
       <c r="AD15" t="inlineStr"/>
       <c r="AE15" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF15" t="inlineStr">
         <is>
-          <t>classificationInformation</t>
+          <t>processInformation/dataSetInformation/classificationInformation</t>
         </is>
       </c>
     </row>
@@ -2091,12 +2091,12 @@
       <c r="AD16" t="inlineStr"/>
       <c r="AE16" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF16" t="inlineStr">
         <is>
-          <t>classification</t>
+          <t>processInformation/dataSetInformation/classification</t>
         </is>
       </c>
     </row>
@@ -2189,12 +2189,12 @@
       <c r="AD17" t="inlineStr"/>
       <c r="AE17" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AF17" t="inlineStr">
         <is>
-          <t>@name</t>
+          <t>processInformation/dataSetInformation/classification/@name</t>
         </is>
       </c>
     </row>
@@ -2287,12 +2287,12 @@
       <c r="AD18" t="inlineStr"/>
       <c r="AE18" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AF18" t="inlineStr">
         <is>
-          <t>@classes</t>
+          <t>processInformation/dataSetInformation/classification/@classes</t>
         </is>
       </c>
     </row>
@@ -2385,12 +2385,12 @@
       <c r="AD19" t="inlineStr"/>
       <c r="AE19" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AF19" t="inlineStr">
         <is>
-          <t>class</t>
+          <t>processInformation/dataSetInformation/classification/class</t>
         </is>
       </c>
     </row>
@@ -2483,12 +2483,12 @@
       <c r="AD20" t="inlineStr"/>
       <c r="AE20" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AF20" t="inlineStr">
         <is>
-          <t>@level</t>
+          <t>processInformation/dataSetInformation/classification/@level</t>
         </is>
       </c>
     </row>
@@ -2581,12 +2581,12 @@
       <c r="AD21" t="inlineStr"/>
       <c r="AE21" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AF21" t="inlineStr">
         <is>
-          <t>@classId</t>
+          <t>processInformation/dataSetInformation/classification/@classId</t>
         </is>
       </c>
     </row>
@@ -2719,12 +2719,12 @@
       <c r="AD22" t="inlineStr"/>
       <c r="AE22" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF22" t="inlineStr">
         <is>
-          <t>generalComment</t>
+          <t>processInformation/dataSetInformation/generalComment</t>
         </is>
       </c>
     </row>
@@ -2849,12 +2849,12 @@
       <c r="AD23" t="inlineStr"/>
       <c r="AE23" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF23" t="inlineStr">
         <is>
-          <t>referenceToExternalDocumentation</t>
+          <t>processInformation/dataSetInformation/referenceToExternalDocumentation</t>
         </is>
       </c>
     </row>
@@ -2943,12 +2943,12 @@
       <c r="AD24" t="inlineStr"/>
       <c r="AE24" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF24" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>processInformation/dataSetInformation/other</t>
         </is>
       </c>
     </row>
@@ -3033,12 +3033,12 @@
       <c r="AD25" t="inlineStr"/>
       <c r="AE25" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AF25" t="inlineStr">
         <is>
-          <t>epd24:referenceServiceLife</t>
+          <t>processInformation/epd24:referenceServiceLife</t>
         </is>
       </c>
     </row>
@@ -3127,12 +3127,12 @@
       <c r="AD26" t="inlineStr"/>
       <c r="AE26" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF26" t="inlineStr">
         <is>
-          <t>@epd24:years</t>
+          <t>processInformation/epd24:referenceServiceLife/@epd24:years</t>
         </is>
       </c>
     </row>
@@ -3217,12 +3217,12 @@
       <c r="AD27" t="inlineStr"/>
       <c r="AE27" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF27" t="inlineStr">
         <is>
-          <t>epd24:useConditionFactor</t>
+          <t>processInformation/epd24:referenceServiceLife/epd24:useConditionFactor</t>
         </is>
       </c>
     </row>
@@ -3318,12 +3318,12 @@
       <c r="AD28" t="inlineStr"/>
       <c r="AE28" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF28" t="inlineStr">
         <is>
-          <t>@epd24:factorCategory</t>
+          <t>processInformation/epd24:referenceServiceLife/@epd24:factorCategory</t>
         </is>
       </c>
     </row>
@@ -3418,12 +3418,12 @@
       <c r="AD29" t="inlineStr"/>
       <c r="AE29" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF29" t="inlineStr">
         <is>
-          <t>@epd24:objectSpecificGrade</t>
+          <t>processInformation/epd24:referenceServiceLife/@epd24:objectSpecificGrade</t>
         </is>
       </c>
     </row>
@@ -3518,12 +3518,12 @@
       <c r="AD30" t="inlineStr"/>
       <c r="AE30" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF30" t="inlineStr">
         <is>
-          <t>@epd24:referenceGrade</t>
+          <t>processInformation/epd24:referenceServiceLife/@epd24:referenceGrade</t>
         </is>
       </c>
     </row>
@@ -3612,12 +3612,12 @@
       <c r="AD31" t="inlineStr"/>
       <c r="AE31" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF31" t="inlineStr">
         <is>
-          <t>@epd24:factor</t>
+          <t>processInformation/epd24:referenceServiceLife/@epd24:factor</t>
         </is>
       </c>
     </row>
@@ -3706,12 +3706,12 @@
       <c r="AD32" t="inlineStr"/>
       <c r="AE32" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF32" t="inlineStr">
         <is>
-          <t>epd24:comment</t>
+          <t>processInformation/epd24:referenceServiceLife/epd24:comment</t>
         </is>
       </c>
     </row>
@@ -3800,12 +3800,12 @@
       <c r="AD33" t="inlineStr"/>
       <c r="AE33" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF33" t="inlineStr">
         <is>
-          <t>epd24:referenceToStandard</t>
+          <t>processInformation/epd24:referenceServiceLife/epd24:referenceToStandard</t>
         </is>
       </c>
     </row>
@@ -3894,12 +3894,12 @@
       <c r="AD34" t="inlineStr"/>
       <c r="AE34" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF34" t="inlineStr">
         <is>
-          <t>epd24:referenceToUseConditionsDocumentation</t>
+          <t>processInformation/epd24:referenceServiceLife/epd24:referenceToUseConditionsDocumentation</t>
         </is>
       </c>
     </row>
@@ -3988,12 +3988,12 @@
       <c r="AD35" t="inlineStr"/>
       <c r="AE35" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF35" t="inlineStr">
         <is>
-          <t>epd24:comment</t>
+          <t>processInformation/epd24:referenceServiceLife/epd24:comment</t>
         </is>
       </c>
     </row>
@@ -4078,12 +4078,12 @@
       <c r="AD36" t="inlineStr"/>
       <c r="AE36" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AF36" t="inlineStr">
         <is>
-          <t>epd24:estimatedServiceLife</t>
+          <t>processInformation/epd24:estimatedServiceLife</t>
         </is>
       </c>
     </row>
@@ -4172,12 +4172,12 @@
       <c r="AD37" t="inlineStr"/>
       <c r="AE37" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF37" t="inlineStr">
         <is>
-          <t>@epd24:years</t>
+          <t>processInformation/epd24:estimatedServiceLife/@epd24:years</t>
         </is>
       </c>
     </row>
@@ -4262,12 +4262,12 @@
       <c r="AD38" t="inlineStr"/>
       <c r="AE38" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF38" t="inlineStr">
         <is>
-          <t>epd24:useConditionFactor</t>
+          <t>processInformation/epd24:estimatedServiceLife/epd24:useConditionFactor</t>
         </is>
       </c>
     </row>
@@ -4363,12 +4363,12 @@
       <c r="AD39" t="inlineStr"/>
       <c r="AE39" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF39" t="inlineStr">
         <is>
-          <t>@epd24:factorCategory</t>
+          <t>processInformation/epd24:estimatedServiceLife/@epd24:factorCategory</t>
         </is>
       </c>
     </row>
@@ -4463,12 +4463,12 @@
       <c r="AD40" t="inlineStr"/>
       <c r="AE40" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF40" t="inlineStr">
         <is>
-          <t>@epd24:objectSpecificGrade</t>
+          <t>processInformation/epd24:estimatedServiceLife/@epd24:objectSpecificGrade</t>
         </is>
       </c>
     </row>
@@ -4563,12 +4563,12 @@
       <c r="AD41" t="inlineStr"/>
       <c r="AE41" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF41" t="inlineStr">
         <is>
-          <t>@epd24:referenceGrade</t>
+          <t>processInformation/epd24:estimatedServiceLife/@epd24:referenceGrade</t>
         </is>
       </c>
     </row>
@@ -4657,12 +4657,12 @@
       <c r="AD42" t="inlineStr"/>
       <c r="AE42" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF42" t="inlineStr">
         <is>
-          <t>@epd24:factor</t>
+          <t>processInformation/epd24:estimatedServiceLife/@epd24:factor</t>
         </is>
       </c>
     </row>
@@ -4751,12 +4751,12 @@
       <c r="AD43" t="inlineStr"/>
       <c r="AE43" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF43" t="inlineStr">
         <is>
-          <t>epd24:comment</t>
+          <t>processInformation/epd24:estimatedServiceLife/epd24:comment</t>
         </is>
       </c>
     </row>
@@ -4845,12 +4845,12 @@
       <c r="AD44" t="inlineStr"/>
       <c r="AE44" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF44" t="inlineStr">
         <is>
-          <t>epd24:referenceToStandard</t>
+          <t>processInformation/epd24:estimatedServiceLife/epd24:referenceToStandard</t>
         </is>
       </c>
     </row>
@@ -4939,12 +4939,12 @@
       <c r="AD45" t="inlineStr"/>
       <c r="AE45" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF45" t="inlineStr">
         <is>
-          <t>epd24:referenceToUseConditionsDocumentation</t>
+          <t>processInformation/epd24:estimatedServiceLife/epd24:referenceToUseConditionsDocumentation</t>
         </is>
       </c>
     </row>
@@ -5033,12 +5033,12 @@
       <c r="AD46" t="inlineStr"/>
       <c r="AE46" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF46" t="inlineStr">
         <is>
-          <t>epd24:comment</t>
+          <t>processInformation/epd24:estimatedServiceLife/epd24:comment</t>
         </is>
       </c>
     </row>
@@ -5119,12 +5119,12 @@
       <c r="AD47" t="inlineStr"/>
       <c r="AE47" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AF47" t="inlineStr">
         <is>
-          <t>epd24:productIds</t>
+          <t>processInformation/epd24:productIds</t>
         </is>
       </c>
     </row>
@@ -5217,12 +5217,12 @@
       <c r="AD48" t="inlineStr"/>
       <c r="AE48" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF48" t="inlineStr">
         <is>
-          <t>epd24:productId</t>
+          <t>processInformation/epd24:productIds/epd24:productId</t>
         </is>
       </c>
     </row>
@@ -5315,12 +5315,12 @@
       <c r="AD49" t="inlineStr"/>
       <c r="AE49" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF49" t="inlineStr">
         <is>
-          <t>@epd24:type</t>
+          <t>processInformation/epd24:productIds/@epd24:type</t>
         </is>
       </c>
     </row>
@@ -5424,12 +5424,12 @@
       <c r="AD50" t="inlineStr"/>
       <c r="AE50" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF50" t="inlineStr">
         <is>
-          <t>epd:safetyMargins</t>
+          <t>processInformation/epd24:productIds/epd:safetyMargins</t>
         </is>
       </c>
     </row>
@@ -5524,12 +5524,12 @@
       <c r="AD51" t="inlineStr"/>
       <c r="AE51" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF51" t="inlineStr">
         <is>
-          <t>epd:margins</t>
+          <t>processInformation/epd24:productIds/epd:margins</t>
         </is>
       </c>
     </row>
@@ -5637,12 +5637,12 @@
       <c r="AD52" t="inlineStr"/>
       <c r="AE52" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF52" t="inlineStr">
         <is>
-          <t>epd:description</t>
+          <t>processInformation/epd24:productIds/epd:description</t>
         </is>
       </c>
     </row>
@@ -5747,12 +5747,12 @@
       <c r="AD53" t="inlineStr"/>
       <c r="AE53" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AF53" t="inlineStr">
         <is>
-          <t>epd:scenarios</t>
+          <t>processInformation/epd:scenarios</t>
         </is>
       </c>
     </row>
@@ -5857,12 +5857,12 @@
       <c r="AD54" t="inlineStr"/>
       <c r="AE54" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF54" t="inlineStr">
         <is>
-          <t>epd:scenario</t>
+          <t>processInformation/epd:scenarios/epd:scenario</t>
         </is>
       </c>
     </row>
@@ -5967,12 +5967,12 @@
       <c r="AD55" t="inlineStr"/>
       <c r="AE55" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF55" t="inlineStr">
         <is>
-          <t>@epd:name</t>
+          <t>processInformation/epd:scenarios/@epd:name</t>
         </is>
       </c>
     </row>
@@ -6061,12 +6061,12 @@
       <c r="AD56" t="inlineStr"/>
       <c r="AE56" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF56" t="inlineStr">
         <is>
-          <t>@epd:default</t>
+          <t>processInformation/epd:scenarios/@epd:default</t>
         </is>
       </c>
     </row>
@@ -6155,12 +6155,12 @@
       <c r="AD57" t="inlineStr"/>
       <c r="AE57" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF57" t="inlineStr">
         <is>
-          <t>@epd:group</t>
+          <t>processInformation/epd:scenarios/@epd:group</t>
         </is>
       </c>
     </row>
@@ -6269,12 +6269,12 @@
       <c r="AD58" t="inlineStr"/>
       <c r="AE58" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF58" t="inlineStr">
         <is>
-          <t>epd:description</t>
+          <t>processInformation/epd:scenarios/epd:description</t>
         </is>
       </c>
     </row>
@@ -6359,12 +6359,12 @@
       <c r="AD59" t="inlineStr"/>
       <c r="AE59" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AF59" t="inlineStr">
         <is>
-          <t>epd:modules</t>
+          <t>processInformation/epd:modules</t>
         </is>
       </c>
     </row>
@@ -6453,12 +6453,12 @@
       <c r="AD60" t="inlineStr"/>
       <c r="AE60" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF60" t="inlineStr">
         <is>
-          <t>epd:module</t>
+          <t>processInformation/epd:modules/epd:module</t>
         </is>
       </c>
     </row>
@@ -6547,12 +6547,12 @@
       <c r="AD61" t="inlineStr"/>
       <c r="AE61" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF61" t="inlineStr">
         <is>
-          <t>@epd:name</t>
+          <t>processInformation/epd:modules/@epd:name</t>
         </is>
       </c>
     </row>
@@ -6641,12 +6641,12 @@
       <c r="AD62" t="inlineStr"/>
       <c r="AE62" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF62" t="inlineStr">
         <is>
-          <t>@epd:productsystem-id</t>
+          <t>processInformation/epd:modules/@epd:productsystem-id</t>
         </is>
       </c>
     </row>
@@ -6762,12 +6762,12 @@
       <c r="AD63" t="inlineStr"/>
       <c r="AE63" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AF63" t="inlineStr">
         <is>
-          <t>epd2:contentDeclaration</t>
+          <t>processInformation/epd2:contentDeclaration</t>
         </is>
       </c>
     </row>
@@ -6852,12 +6852,12 @@
       <c r="AD64" t="inlineStr"/>
       <c r="AE64" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF64" t="inlineStr">
         <is>
-          <t>epd2:component</t>
+          <t>processInformation/epd2:contentDeclaration/epd2:component</t>
         </is>
       </c>
     </row>
@@ -6946,12 +6946,12 @@
       <c r="AD65" t="inlineStr"/>
       <c r="AE65" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF65" t="inlineStr">
         <is>
-          <t>epd2:name</t>
+          <t>processInformation/epd2:contentDeclaration/epd2:name</t>
         </is>
       </c>
     </row>
@@ -7036,12 +7036,12 @@
       <c r="AD66" t="inlineStr"/>
       <c r="AE66" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF66" t="inlineStr">
         <is>
-          <t>epd2:weightPerc</t>
+          <t>processInformation/epd2:contentDeclaration/epd2:weightPerc</t>
         </is>
       </c>
     </row>
@@ -7126,12 +7126,12 @@
       <c r="AD67" t="inlineStr"/>
       <c r="AE67" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF67" t="inlineStr">
         <is>
-          <t>@epd2:value</t>
+          <t>processInformation/epd2:contentDeclaration/@epd2:value</t>
         </is>
       </c>
     </row>
@@ -7216,12 +7216,12 @@
       <c r="AD68" t="inlineStr"/>
       <c r="AE68" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF68" t="inlineStr">
         <is>
-          <t>@epd2:lowerValue</t>
+          <t>processInformation/epd2:contentDeclaration/@epd2:lowerValue</t>
         </is>
       </c>
     </row>
@@ -7306,12 +7306,12 @@
       <c r="AD69" t="inlineStr"/>
       <c r="AE69" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF69" t="inlineStr">
         <is>
-          <t>@epd2:upperValue</t>
+          <t>processInformation/epd2:contentDeclaration/@epd2:upperValue</t>
         </is>
       </c>
     </row>
@@ -7396,12 +7396,12 @@
       <c r="AD70" t="inlineStr"/>
       <c r="AE70" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF70" t="inlineStr">
         <is>
-          <t>epd2:mass</t>
+          <t>processInformation/epd2:contentDeclaration/epd2:mass</t>
         </is>
       </c>
     </row>
@@ -7486,12 +7486,12 @@
       <c r="AD71" t="inlineStr"/>
       <c r="AE71" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF71" t="inlineStr">
         <is>
-          <t>@epd2:value</t>
+          <t>processInformation/epd2:contentDeclaration/@epd2:value</t>
         </is>
       </c>
     </row>
@@ -7576,12 +7576,12 @@
       <c r="AD72" t="inlineStr"/>
       <c r="AE72" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF72" t="inlineStr">
         <is>
-          <t>@epd2:lowerValue</t>
+          <t>processInformation/epd2:contentDeclaration/@epd2:lowerValue</t>
         </is>
       </c>
     </row>
@@ -7666,12 +7666,12 @@
       <c r="AD73" t="inlineStr"/>
       <c r="AE73" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF73" t="inlineStr">
         <is>
-          <t>@epd2:upperValue</t>
+          <t>processInformation/epd2:contentDeclaration/@epd2:upperValue</t>
         </is>
       </c>
     </row>
@@ -7764,12 +7764,12 @@
       <c r="AD74" t="inlineStr"/>
       <c r="AE74" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF74" t="inlineStr">
         <is>
-          <t>epd2:comment</t>
+          <t>processInformation/epd2:contentDeclaration/epd2:comment</t>
         </is>
       </c>
     </row>
@@ -7854,12 +7854,12 @@
       <c r="AD75" t="inlineStr"/>
       <c r="AE75" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF75" t="inlineStr">
         <is>
-          <t>epd2:material_|_epd2:substance</t>
+          <t>processInformation/epd2:contentDeclaration/epd2:material_|_epd2:substance</t>
         </is>
       </c>
     </row>
@@ -7948,12 +7948,12 @@
       <c r="AD76" t="inlineStr"/>
       <c r="AE76" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF76" t="inlineStr">
         <is>
-          <t>epd2:name</t>
+          <t>processInformation/epd2:contentDeclaration/epd2:name</t>
         </is>
       </c>
     </row>
@@ -8038,12 +8038,12 @@
       <c r="AD77" t="inlineStr"/>
       <c r="AE77" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF77" t="inlineStr">
         <is>
-          <t>epd2:weightPerc</t>
+          <t>processInformation/epd2:contentDeclaration/epd2:weightPerc</t>
         </is>
       </c>
     </row>
@@ -8128,12 +8128,12 @@
       <c r="AD78" t="inlineStr"/>
       <c r="AE78" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF78" t="inlineStr">
         <is>
-          <t>@epd2:value</t>
+          <t>processInformation/epd2:contentDeclaration/@epd2:value</t>
         </is>
       </c>
     </row>
@@ -8218,12 +8218,12 @@
       <c r="AD79" t="inlineStr"/>
       <c r="AE79" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF79" t="inlineStr">
         <is>
-          <t>@epd2:lowerValue</t>
+          <t>processInformation/epd2:contentDeclaration/@epd2:lowerValue</t>
         </is>
       </c>
     </row>
@@ -8308,12 +8308,12 @@
       <c r="AD80" t="inlineStr"/>
       <c r="AE80" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF80" t="inlineStr">
         <is>
-          <t>@epd2:upperValue</t>
+          <t>processInformation/epd2:contentDeclaration/@epd2:upperValue</t>
         </is>
       </c>
     </row>
@@ -8398,12 +8398,12 @@
       <c r="AD81" t="inlineStr"/>
       <c r="AE81" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF81" t="inlineStr">
         <is>
-          <t>epd2:mass</t>
+          <t>processInformation/epd2:contentDeclaration/epd2:mass</t>
         </is>
       </c>
     </row>
@@ -8488,12 +8488,12 @@
       <c r="AD82" t="inlineStr"/>
       <c r="AE82" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF82" t="inlineStr">
         <is>
-          <t>@epd2:value</t>
+          <t>processInformation/epd2:contentDeclaration/@epd2:value</t>
         </is>
       </c>
     </row>
@@ -8578,12 +8578,12 @@
       <c r="AD83" t="inlineStr"/>
       <c r="AE83" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF83" t="inlineStr">
         <is>
-          <t>@epd2:lowerValue</t>
+          <t>processInformation/epd2:contentDeclaration/@epd2:lowerValue</t>
         </is>
       </c>
     </row>
@@ -8668,12 +8668,12 @@
       <c r="AD84" t="inlineStr"/>
       <c r="AE84" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF84" t="inlineStr">
         <is>
-          <t>@epd2:upperValue</t>
+          <t>processInformation/epd2:contentDeclaration/@epd2:upperValue</t>
         </is>
       </c>
     </row>
@@ -8758,12 +8758,12 @@
       <c r="AD85" t="inlineStr"/>
       <c r="AE85" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF85" t="inlineStr">
         <is>
-          <t>@epd2:CASNumber</t>
+          <t>processInformation/epd2:contentDeclaration/@epd2:CASNumber</t>
         </is>
       </c>
     </row>
@@ -8848,12 +8848,12 @@
       <c r="AD86" t="inlineStr"/>
       <c r="AE86" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF86" t="inlineStr">
         <is>
-          <t>@epd2:ECNumber</t>
+          <t>processInformation/epd2:contentDeclaration/@epd2:ECNumber</t>
         </is>
       </c>
     </row>
@@ -8938,12 +8938,12 @@
       <c r="AD87" t="inlineStr"/>
       <c r="AE87" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF87" t="inlineStr">
         <is>
-          <t>@epd2:hazardCode</t>
+          <t>processInformation/epd2:contentDeclaration/@epd2:hazardCode</t>
         </is>
       </c>
     </row>
@@ -9028,12 +9028,12 @@
       <c r="AD88" t="inlineStr"/>
       <c r="AE88" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF88" t="inlineStr">
         <is>
-          <t>@epd2:renewable</t>
+          <t>processInformation/epd2:contentDeclaration/@epd2:renewable</t>
         </is>
       </c>
     </row>
@@ -9118,12 +9118,12 @@
       <c r="AD89" t="inlineStr"/>
       <c r="AE89" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF89" t="inlineStr">
         <is>
-          <t>@epd2:recycled</t>
+          <t>processInformation/epd2:contentDeclaration/@epd2:recycled</t>
         </is>
       </c>
     </row>
@@ -9208,12 +9208,12 @@
       <c r="AD90" t="inlineStr"/>
       <c r="AE90" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF90" t="inlineStr">
         <is>
-          <t>@epd2:recyclable</t>
+          <t>processInformation/epd2:contentDeclaration/@epd2:recyclable</t>
         </is>
       </c>
     </row>
@@ -9298,12 +9298,12 @@
       <c r="AD91" t="inlineStr"/>
       <c r="AE91" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF91" t="inlineStr">
         <is>
-          <t>@epd2:packaging</t>
+          <t>processInformation/epd2:contentDeclaration/@epd2:packaging</t>
         </is>
       </c>
     </row>
@@ -9392,12 +9392,12 @@
       <c r="AD92" t="inlineStr"/>
       <c r="AE92" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF92" t="inlineStr">
         <is>
-          <t>epd2:comment</t>
+          <t>processInformation/epd2:contentDeclaration/epd2:comment</t>
         </is>
       </c>
     </row>
@@ -9486,12 +9486,12 @@
       <c r="AD93" t="inlineStr"/>
       <c r="AE93" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF93" t="inlineStr">
         <is>
-          <t>epd24:SVHC</t>
+          <t>processInformation/epd2:contentDeclaration/epd24:SVHC</t>
         </is>
       </c>
     </row>
@@ -9576,12 +9576,12 @@
       <c r="AD94" t="inlineStr"/>
       <c r="AE94" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AF94" t="inlineStr">
         <is>
-          <t>epd24:scenarioData</t>
+          <t>processInformation/epd24:scenarioData</t>
         </is>
       </c>
     </row>
@@ -9666,12 +9666,12 @@
       <c r="AD95" t="inlineStr"/>
       <c r="AE95" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF95" t="inlineStr">
         <is>
-          <t>epd24:useStageScenarioData</t>
+          <t>processInformation/epd24:scenarioData/epd24:useStageScenarioData</t>
         </is>
       </c>
     </row>
@@ -9760,12 +9760,12 @@
       <c r="AD96" t="inlineStr"/>
       <c r="AE96" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF96" t="inlineStr">
         <is>
-          <t>@epd24:scenario</t>
+          <t>processInformation/epd24:scenarioData/@epd24:scenario</t>
         </is>
       </c>
     </row>
@@ -9863,12 +9863,12 @@
       <c r="AD97" t="inlineStr"/>
       <c r="AE97" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AF97" t="inlineStr">
         <is>
-          <t>epd24:soilAndWaterImpacts</t>
+          <t>processInformation/epd24:soilAndWaterImpacts</t>
         </is>
       </c>
     </row>
@@ -9961,12 +9961,12 @@
       <c r="AD98" t="inlineStr"/>
       <c r="AE98" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF98" t="inlineStr">
         <is>
-          <t>epd24:soilAndWaterImpactsDescription</t>
+          <t>processInformation/epd24:soilAndWaterImpacts/epd24:soilAndWaterImpactsDescription</t>
         </is>
       </c>
     </row>
@@ -10069,12 +10069,12 @@
       <c r="AD99" t="inlineStr"/>
       <c r="AE99" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AF99" t="inlineStr">
         <is>
-          <t>epd24:eolScenarioData</t>
+          <t>processInformation/epd24:eolScenarioData</t>
         </is>
       </c>
     </row>
@@ -10163,12 +10163,12 @@
       <c r="AD100" t="inlineStr"/>
       <c r="AE100" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF100" t="inlineStr">
         <is>
-          <t>@epd24:scenario</t>
+          <t>processInformation/epd24:eolScenarioData/@epd24:scenario</t>
         </is>
       </c>
     </row>
@@ -10253,12 +10253,12 @@
       <c r="AD101" t="inlineStr"/>
       <c r="AE101" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF101" t="inlineStr">
         <is>
-          <t>epd24:collection</t>
+          <t>processInformation/epd24:eolScenarioData/epd24:collection</t>
         </is>
       </c>
     </row>
@@ -10347,12 +10347,12 @@
       <c r="AD102" t="inlineStr"/>
       <c r="AE102" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF102" t="inlineStr">
         <is>
-          <t>@epd24:separate</t>
+          <t>processInformation/epd24:eolScenarioData/@epd24:separate</t>
         </is>
       </c>
     </row>
@@ -10441,12 +10441,12 @@
       <c r="AD103" t="inlineStr"/>
       <c r="AE103" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF103" t="inlineStr">
         <is>
-          <t>@epd24:withMixedWaste</t>
+          <t>processInformation/epd24:eolScenarioData/@epd24:withMixedWaste</t>
         </is>
       </c>
     </row>
@@ -10531,12 +10531,12 @@
       <c r="AD104" t="inlineStr"/>
       <c r="AE104" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF104" t="inlineStr">
         <is>
-          <t>epd24:recovery</t>
+          <t>processInformation/epd24:eolScenarioData/epd24:recovery</t>
         </is>
       </c>
     </row>
@@ -10625,12 +10625,12 @@
       <c r="AD105" t="inlineStr"/>
       <c r="AE105" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF105" t="inlineStr">
         <is>
-          <t>@epd24:reuse</t>
+          <t>processInformation/epd24:eolScenarioData/@epd24:reuse</t>
         </is>
       </c>
     </row>
@@ -10719,12 +10719,12 @@
       <c r="AD106" t="inlineStr"/>
       <c r="AE106" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF106" t="inlineStr">
         <is>
-          <t>@epd24:recycling</t>
+          <t>processInformation/epd24:eolScenarioData/@epd24:recycling</t>
         </is>
       </c>
     </row>
@@ -10813,12 +10813,12 @@
       <c r="AD107" t="inlineStr"/>
       <c r="AE107" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF107" t="inlineStr">
         <is>
-          <t>@epd24:energyRecovery</t>
+          <t>processInformation/epd24:eolScenarioData/@epd24:energyRecovery</t>
         </is>
       </c>
     </row>
@@ -10903,12 +10903,12 @@
       <c r="AD108" t="inlineStr"/>
       <c r="AE108" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF108" t="inlineStr">
         <is>
-          <t>epd24:disposal</t>
+          <t>processInformation/epd24:eolScenarioData/epd24:disposal</t>
         </is>
       </c>
     </row>
@@ -10997,12 +10997,12 @@
       <c r="AD109" t="inlineStr"/>
       <c r="AE109" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF109" t="inlineStr">
         <is>
-          <t>@epd24:finalDeposition</t>
+          <t>processInformation/epd24:eolScenarioData/@epd24:finalDeposition</t>
         </is>
       </c>
     </row>
@@ -11087,12 +11087,12 @@
       <c r="AD110" t="inlineStr"/>
       <c r="AE110" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AF110" t="inlineStr">
         <is>
-          <t>quantitativeReference</t>
+          <t>processInformation/quantitativeReference</t>
         </is>
       </c>
     </row>
@@ -11193,12 +11193,12 @@
       <c r="AD111" t="inlineStr"/>
       <c r="AE111" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF111" t="inlineStr">
         <is>
-          <t>@type</t>
+          <t>processInformation/quantitativeReference/@type</t>
         </is>
       </c>
     </row>
@@ -11315,12 +11315,12 @@
       <c r="AD112" t="inlineStr"/>
       <c r="AE112" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF112" t="inlineStr">
         <is>
-          <t>referenceToReferenceFlow</t>
+          <t>processInformation/quantitativeReference/referenceToReferenceFlow</t>
         </is>
       </c>
     </row>
@@ -11425,12 +11425,12 @@
       <c r="AD113" t="inlineStr"/>
       <c r="AE113" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF113" t="inlineStr">
         <is>
-          <t>functionalUnitOrOther</t>
+          <t>processInformation/quantitativeReference/functionalUnitOrOther</t>
         </is>
       </c>
     </row>
@@ -11519,12 +11519,12 @@
       <c r="AD114" t="inlineStr"/>
       <c r="AE114" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF114" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>processInformation/quantitativeReference/other</t>
         </is>
       </c>
     </row>
@@ -11609,12 +11609,12 @@
       <c r="AD115" t="inlineStr"/>
       <c r="AE115" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AF115" t="inlineStr">
         <is>
-          <t>time</t>
+          <t>processInformation/time</t>
         </is>
       </c>
     </row>
@@ -11719,12 +11719,12 @@
       <c r="AD116" t="inlineStr"/>
       <c r="AE116" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF116" t="inlineStr">
         <is>
-          <t>referenceYear</t>
+          <t>processInformation/time/referenceYear</t>
         </is>
       </c>
     </row>
@@ -11837,12 +11837,12 @@
       <c r="AD117" t="inlineStr"/>
       <c r="AE117" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF117" t="inlineStr">
         <is>
-          <t>dataSetValidUntil</t>
+          <t>processInformation/time/dataSetValidUntil</t>
         </is>
       </c>
     </row>
@@ -11943,12 +11943,12 @@
       <c r="AD118" t="inlineStr"/>
       <c r="AE118" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF118" t="inlineStr">
         <is>
-          <t>timeRepresentativenessDescription</t>
+          <t>processInformation/time/timeRepresentativenessDescription</t>
         </is>
       </c>
     </row>
@@ -12037,12 +12037,12 @@
       <c r="AD119" t="inlineStr"/>
       <c r="AE119" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF119" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>processInformation/time/other</t>
         </is>
       </c>
     </row>
@@ -12155,12 +12155,12 @@
       <c r="AD120" t="inlineStr"/>
       <c r="AE120" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AF120" t="inlineStr">
         <is>
-          <t>epd2:publicationDateOfEPD</t>
+          <t>processInformation/time/other/epd2:publicationDateOfEPD</t>
         </is>
       </c>
     </row>
@@ -12249,12 +12249,12 @@
       <c r="AD121" t="inlineStr"/>
       <c r="AE121" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF121" t="inlineStr">
         <is>
-          <t>epd2:expirationDateOfEPD</t>
+          <t>processInformation/time/epd2:expirationDateOfEPD</t>
         </is>
       </c>
     </row>
@@ -12343,12 +12343,12 @@
       <c r="AD122" t="inlineStr"/>
       <c r="AE122" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AF122" t="inlineStr">
         <is>
-          <t>geography</t>
+          <t>processInformation/geography</t>
         </is>
       </c>
     </row>
@@ -12437,12 +12437,12 @@
       <c r="AD123" t="inlineStr"/>
       <c r="AE123" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF123" t="inlineStr">
         <is>
-          <t>locationOfOperationSupplyOrProduction</t>
+          <t>processInformation/geography/locationOfOperationSupplyOrProduction</t>
         </is>
       </c>
     </row>
@@ -12555,12 +12555,12 @@
       <c r="AD124" t="inlineStr"/>
       <c r="AE124" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF124" t="inlineStr">
         <is>
-          <t>@location</t>
+          <t>processInformation/geography/@location</t>
         </is>
       </c>
     </row>
@@ -12670,12 +12670,12 @@
       <c r="AD125" t="inlineStr"/>
       <c r="AE125" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF125" t="inlineStr">
         <is>
-          <t>descriptionOfRestrictions</t>
+          <t>processInformation/geography/descriptionOfRestrictions</t>
         </is>
       </c>
     </row>
@@ -12764,12 +12764,12 @@
       <c r="AD126" t="inlineStr"/>
       <c r="AE126" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF126" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>processInformation/geography/other</t>
         </is>
       </c>
     </row>
@@ -12858,12 +12858,12 @@
       <c r="AD127" t="inlineStr"/>
       <c r="AE127" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AF127" t="inlineStr">
         <is>
-          <t>technology</t>
+          <t>processInformation/technology</t>
         </is>
       </c>
     </row>
@@ -13004,12 +13004,12 @@
       <c r="AD128" t="inlineStr"/>
       <c r="AE128" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF128" t="inlineStr">
         <is>
-          <t>technologyDescriptionAndIncludedProcesses</t>
+          <t>processInformation/technology/technologyDescriptionAndIncludedProcesses</t>
         </is>
       </c>
     </row>
@@ -13140,12 +13140,12 @@
       <c r="AD129" t="inlineStr"/>
       <c r="AE129" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF129" t="inlineStr">
         <is>
-          <t>technologicalApplicability</t>
+          <t>processInformation/technology/technologicalApplicability</t>
         </is>
       </c>
     </row>
@@ -13251,12 +13251,12 @@
       <c r="AD130" t="inlineStr"/>
       <c r="AE130" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF130" t="inlineStr">
         <is>
-          <t>referenceToTechnologyPictogramme</t>
+          <t>processInformation/technology/referenceToTechnologyPictogramme</t>
         </is>
       </c>
     </row>
@@ -13378,12 +13378,12 @@
       <c r="AD131" t="inlineStr"/>
       <c r="AE131" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF131" t="inlineStr">
         <is>
-          <t>referenceToTechnologyFlowDiagrammOrPicture</t>
+          <t>processInformation/technology/referenceToTechnologyFlowDiagrammOrPicture</t>
         </is>
       </c>
     </row>
@@ -13472,12 +13472,12 @@
       <c r="AD132" t="inlineStr"/>
       <c r="AE132" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF132" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>processInformation/technology/other</t>
         </is>
       </c>
     </row>
@@ -13660,12 +13660,12 @@
       <c r="AD134" t="inlineStr"/>
       <c r="AE134" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AF134" t="inlineStr">
         <is>
-          <t>LCIMethodAndAllocation</t>
+          <t>modellingAndValidation/LCIMethodAndAllocation</t>
         </is>
       </c>
     </row>
@@ -13762,12 +13762,12 @@
       <c r="AD135" t="inlineStr"/>
       <c r="AE135" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF135" t="inlineStr">
         <is>
-          <t>typeOfDataSet</t>
+          <t>modellingAndValidation/LCIMethodAndAllocation/typeOfDataSet</t>
         </is>
       </c>
     </row>
@@ -13899,12 +13899,12 @@
       <c r="AD136" t="inlineStr"/>
       <c r="AE136" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF136" t="inlineStr">
         <is>
-          <t>referenceToLCAMethodDetails</t>
+          <t>modellingAndValidation/LCIMethodAndAllocation/referenceToLCAMethodDetails</t>
         </is>
       </c>
     </row>
@@ -14023,12 +14023,12 @@
       <c r="AD137" t="inlineStr"/>
       <c r="AE137" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF137" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>modellingAndValidation/LCIMethodAndAllocation/other</t>
         </is>
       </c>
     </row>
@@ -14156,12 +14156,12 @@
       <c r="AD138" t="inlineStr"/>
       <c r="AE138" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AF138" t="inlineStr">
         <is>
-          <t>epd:subType</t>
+          <t>modellingAndValidation/LCIMethodAndAllocation/other/epd:subType</t>
         </is>
       </c>
     </row>
@@ -14246,12 +14246,12 @@
       <c r="AD139" t="inlineStr"/>
       <c r="AE139" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF139" t="inlineStr">
         <is>
-          <t>epd24:pcrCompliance</t>
+          <t>modellingAndValidation/LCIMethodAndAllocation/epd24:pcrCompliance</t>
         </is>
       </c>
     </row>
@@ -14340,12 +14340,12 @@
       <c r="AD140" t="inlineStr"/>
       <c r="AE140" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF140" t="inlineStr">
         <is>
-          <t>@epd24:allocation</t>
+          <t>modellingAndValidation/LCIMethodAndAllocation/@epd24:allocation</t>
         </is>
       </c>
     </row>
@@ -14444,12 +14444,12 @@
       <c r="AD141" t="inlineStr"/>
       <c r="AE141" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF141" t="inlineStr">
         <is>
-          <t>@epd24:cutOffRules</t>
+          <t>modellingAndValidation/LCIMethodAndAllocation/@epd24:cutOffRules</t>
         </is>
       </c>
     </row>
@@ -14550,12 +14550,12 @@
       <c r="AD142" t="inlineStr"/>
       <c r="AE142" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF142" t="inlineStr">
         <is>
-          <t>@epd24:upstreamDataDeviatingFromAllocationPrinciples</t>
+          <t>modellingAndValidation/LCIMethodAndAllocation/@epd24:upstreamDataDeviatingFromAllocationPrinciples</t>
         </is>
       </c>
     </row>
@@ -14669,12 +14669,12 @@
       <c r="AD143" t="inlineStr"/>
       <c r="AE143" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF143" t="inlineStr">
         <is>
-          <t>epd24:variability</t>
+          <t>modellingAndValidation/LCIMethodAndAllocation/epd24:variability</t>
         </is>
       </c>
     </row>
@@ -14771,12 +14771,12 @@
       <c r="AD144" t="inlineStr"/>
       <c r="AE144" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF144" t="inlineStr">
         <is>
-          <t>epd24:manufacturerVariability</t>
+          <t>modellingAndValidation/LCIMethodAndAllocation/epd24:manufacturerVariability</t>
         </is>
       </c>
     </row>
@@ -14867,12 +14867,12 @@
       <c r="AD145" t="inlineStr"/>
       <c r="AE145" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF145" t="inlineStr">
         <is>
-          <t>@epd24:type</t>
+          <t>modellingAndValidation/LCIMethodAndAllocation/@epd24:type</t>
         </is>
       </c>
     </row>
@@ -14961,12 +14961,12 @@
       <c r="AD146" t="inlineStr"/>
       <c r="AE146" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF146" t="inlineStr">
         <is>
-          <t>@epd24:variation</t>
+          <t>modellingAndValidation/LCIMethodAndAllocation/@epd24:variation</t>
         </is>
       </c>
     </row>
@@ -15060,12 +15060,12 @@
       <c r="AD147" t="inlineStr"/>
       <c r="AE147" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF147" t="inlineStr">
         <is>
-          <t>@epd24:variationRange</t>
+          <t>modellingAndValidation/LCIMethodAndAllocation/@epd24:variationRange</t>
         </is>
       </c>
     </row>
@@ -15162,12 +15162,12 @@
       <c r="AD148" t="inlineStr"/>
       <c r="AE148" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF148" t="inlineStr">
         <is>
-          <t>epd24:productVariability</t>
+          <t>modellingAndValidation/LCIMethodAndAllocation/epd24:productVariability</t>
         </is>
       </c>
     </row>
@@ -15257,12 +15257,12 @@
       <c r="AD149" t="inlineStr"/>
       <c r="AE149" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF149" t="inlineStr">
         <is>
-          <t>@epd24:type</t>
+          <t>modellingAndValidation/LCIMethodAndAllocation/@epd24:type</t>
         </is>
       </c>
     </row>
@@ -15351,12 +15351,12 @@
       <c r="AD150" t="inlineStr"/>
       <c r="AE150" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF150" t="inlineStr">
         <is>
-          <t>@epd24:variation</t>
+          <t>modellingAndValidation/LCIMethodAndAllocation/@epd24:variation</t>
         </is>
       </c>
     </row>
@@ -15450,12 +15450,12 @@
       <c r="AD151" t="inlineStr"/>
       <c r="AE151" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF151" t="inlineStr">
         <is>
-          <t>@epd24:variationRange</t>
+          <t>modellingAndValidation/LCIMethodAndAllocation/@epd24:variationRange</t>
         </is>
       </c>
     </row>
@@ -15544,12 +15544,12 @@
       <c r="AD152" t="inlineStr"/>
       <c r="AE152" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF152" t="inlineStr">
         <is>
-          <t>epd24:variabilityDescription</t>
+          <t>modellingAndValidation/LCIMethodAndAllocation/epd24:variabilityDescription</t>
         </is>
       </c>
     </row>
@@ -15656,12 +15656,12 @@
       <c r="AD153" t="inlineStr"/>
       <c r="AE153" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF153" t="inlineStr">
         <is>
-          <t>epd:safetyMargins</t>
+          <t>modellingAndValidation/LCIMethodAndAllocation/epd:safetyMargins</t>
         </is>
       </c>
     </row>
@@ -15759,12 +15759,12 @@
       <c r="AD154" t="inlineStr"/>
       <c r="AE154" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF154" t="inlineStr">
         <is>
-          <t>epd:margins</t>
+          <t>modellingAndValidation/LCIMethodAndAllocation/epd:margins</t>
         </is>
       </c>
     </row>
@@ -15875,12 +15875,12 @@
       <c r="AD155" t="inlineStr"/>
       <c r="AE155" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF155" t="inlineStr">
         <is>
-          <t>epd:description</t>
+          <t>modellingAndValidation/LCIMethodAndAllocation/epd:description</t>
         </is>
       </c>
     </row>
@@ -15969,12 +15969,12 @@
       <c r="AD156" t="inlineStr"/>
       <c r="AE156" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AF156" t="inlineStr">
         <is>
-          <t>dataSourcesTreatmentAndRepresentativeness</t>
+          <t>modellingAndValidation/dataSourcesTreatmentAndRepresentativeness</t>
         </is>
       </c>
     </row>
@@ -16088,12 +16088,12 @@
       <c r="AD157" t="inlineStr"/>
       <c r="AE157" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF157" t="inlineStr">
         <is>
-          <t>referenceToDataHandlingPrinciples</t>
+          <t>modellingAndValidation/dataSourcesTreatmentAndRepresentativeness/referenceToDataHandlingPrinciples</t>
         </is>
       </c>
     </row>
@@ -16231,12 +16231,12 @@
       <c r="AD158" t="inlineStr"/>
       <c r="AE158" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF158" t="inlineStr">
         <is>
-          <t>referenceToDataSource</t>
+          <t>modellingAndValidation/dataSourcesTreatmentAndRepresentativeness/referenceToDataSource</t>
         </is>
       </c>
     </row>
@@ -16367,12 +16367,12 @@
       <c r="AD159" t="inlineStr"/>
       <c r="AE159" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF159" t="inlineStr">
         <is>
-          <t>useAdviceForDataSet</t>
+          <t>modellingAndValidation/dataSourcesTreatmentAndRepresentativeness/useAdviceForDataSet</t>
         </is>
       </c>
     </row>
@@ -16461,12 +16461,12 @@
       <c r="AD160" t="inlineStr"/>
       <c r="AE160" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF160" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>modellingAndValidation/dataSourcesTreatmentAndRepresentativeness/other</t>
         </is>
       </c>
     </row>
@@ -16568,12 +16568,12 @@
       <c r="AD161" t="inlineStr"/>
       <c r="AE161" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF161" t="inlineStr">
         <is>
-          <t>epd2:referenceToOriginalEPD</t>
+          <t>modellingAndValidation/dataSourcesTreatmentAndRepresentativeness/epd2:referenceToOriginalEPD</t>
         </is>
       </c>
     </row>
@@ -16678,12 +16678,12 @@
       <c r="AD162" t="inlineStr"/>
       <c r="AE162" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AF162" t="inlineStr">
         <is>
-          <t>epd24:manufacturers</t>
+          <t>modellingAndValidation/epd24:manufacturers</t>
         </is>
       </c>
     </row>
@@ -16784,12 +16784,12 @@
       <c r="AD163" t="inlineStr"/>
       <c r="AE163" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF163" t="inlineStr">
         <is>
-          <t>epd24:manufacturer</t>
+          <t>modellingAndValidation/epd24:manufacturers/epd24:manufacturer</t>
         </is>
       </c>
     </row>
@@ -16894,12 +16894,12 @@
       <c r="AD164" t="inlineStr"/>
       <c r="AE164" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF164" t="inlineStr">
         <is>
-          <t>epd24:contact</t>
+          <t>modellingAndValidation/epd24:manufacturers/epd24:contact</t>
         </is>
       </c>
     </row>
@@ -17004,12 +17004,12 @@
       <c r="AD165" t="inlineStr"/>
       <c r="AE165" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF165" t="inlineStr">
         <is>
-          <t>epd24:sites</t>
+          <t>modellingAndValidation/epd24:manufacturers/epd24:sites</t>
         </is>
       </c>
     </row>
@@ -17110,12 +17110,12 @@
       <c r="AD166" t="inlineStr"/>
       <c r="AE166" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF166" t="inlineStr">
         <is>
-          <t>epd24:site</t>
+          <t>modellingAndValidation/epd24:manufacturers/epd24:site</t>
         </is>
       </c>
     </row>
@@ -17220,12 +17220,12 @@
       <c r="AD167" t="inlineStr"/>
       <c r="AE167" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF167" t="inlineStr">
         <is>
-          <t>epd24:name</t>
+          <t>modellingAndValidation/epd24:manufacturers/epd24:name</t>
         </is>
       </c>
     </row>
@@ -17330,12 +17330,12 @@
       <c r="AD168" t="inlineStr"/>
       <c r="AE168" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF168" t="inlineStr">
         <is>
-          <t>epd24:facilityIdentifier</t>
+          <t>modellingAndValidation/epd24:manufacturers/epd24:facilityIdentifier</t>
         </is>
       </c>
     </row>
@@ -17444,12 +17444,12 @@
       <c r="AD169" t="inlineStr"/>
       <c r="AE169" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF169" t="inlineStr">
         <is>
-          <t>epd24:olc</t>
+          <t>modellingAndValidation/epd24:manufacturers/epd24:olc</t>
         </is>
       </c>
     </row>
@@ -17554,12 +17554,12 @@
       <c r="AD170" t="inlineStr"/>
       <c r="AE170" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF170" t="inlineStr">
         <is>
-          <t>epd24:geoCode</t>
+          <t>modellingAndValidation/epd24:manufacturers/epd24:geoCode</t>
         </is>
       </c>
     </row>
@@ -17664,12 +17664,12 @@
       <c r="AD171" t="inlineStr"/>
       <c r="AE171" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF171" t="inlineStr">
         <is>
-          <t>epd24:streetAddress</t>
+          <t>modellingAndValidation/epd24:manufacturers/epd24:streetAddress</t>
         </is>
       </c>
     </row>
@@ -17763,12 +17763,12 @@
       <c r="AD172" t="inlineStr"/>
       <c r="AE172" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF172" t="inlineStr">
         <is>
-          <t>epd2:referenceToOriginalEPD</t>
+          <t>modellingAndValidation/epd24:manufacturers/epd2:referenceToOriginalEPD</t>
         </is>
       </c>
     </row>
@@ -17869,12 +17869,12 @@
       <c r="AD173" t="inlineStr"/>
       <c r="AE173" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AF173" t="inlineStr">
         <is>
-          <t>validation</t>
+          <t>modellingAndValidation/validation</t>
         </is>
       </c>
     </row>
@@ -17967,12 +17967,12 @@
       <c r="AD174" t="inlineStr"/>
       <c r="AE174" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF174" t="inlineStr">
         <is>
-          <t>review</t>
+          <t>modellingAndValidation/validation/review</t>
         </is>
       </c>
     </row>
@@ -18120,12 +18120,12 @@
       <c r="AD175" t="inlineStr"/>
       <c r="AE175" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF175" t="inlineStr">
         <is>
-          <t>@type</t>
+          <t>modellingAndValidation/validation/@type</t>
         </is>
       </c>
     </row>
@@ -18238,12 +18238,12 @@
       <c r="AD176" t="inlineStr"/>
       <c r="AE176" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF176" t="inlineStr">
         <is>
-          <t>reviewDetails</t>
+          <t>modellingAndValidation/validation/reviewDetails</t>
         </is>
       </c>
     </row>
@@ -18371,12 +18371,12 @@
       <c r="AD177" t="inlineStr"/>
       <c r="AE177" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF177" t="inlineStr">
         <is>
-          <t>referenceToNameOfReviewerAndInstitution</t>
+          <t>modellingAndValidation/validation/referenceToNameOfReviewerAndInstitution</t>
         </is>
       </c>
     </row>
@@ -18477,12 +18477,12 @@
       <c r="AD178" t="inlineStr"/>
       <c r="AE178" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF178" t="inlineStr">
         <is>
-          <t>referenceToCompleteReviewReport</t>
+          <t>modellingAndValidation/validation/referenceToCompleteReviewReport</t>
         </is>
       </c>
     </row>
@@ -18571,12 +18571,12 @@
       <c r="AD179" t="inlineStr"/>
       <c r="AE179" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF179" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>modellingAndValidation/validation/other</t>
         </is>
       </c>
     </row>
@@ -18665,12 +18665,12 @@
       <c r="AD180" t="inlineStr"/>
       <c r="AE180" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AF180" t="inlineStr">
         <is>
-          <t>complianceDeclarations</t>
+          <t>modellingAndValidation/complianceDeclarations</t>
         </is>
       </c>
     </row>
@@ -18763,12 +18763,12 @@
       <c r="AD181" t="inlineStr"/>
       <c r="AE181" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF181" t="inlineStr">
         <is>
-          <t>compliance</t>
+          <t>modellingAndValidation/complianceDeclarations/compliance</t>
         </is>
       </c>
     </row>
@@ -18894,12 +18894,12 @@
       <c r="AD182" t="inlineStr"/>
       <c r="AE182" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF182" t="inlineStr">
         <is>
-          <t>referenceToComplianceSystem</t>
+          <t>modellingAndValidation/complianceDeclarations/referenceToComplianceSystem</t>
         </is>
       </c>
     </row>
@@ -18988,12 +18988,12 @@
       <c r="AD183" t="inlineStr"/>
       <c r="AE183" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF183" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>modellingAndValidation/complianceDeclarations/other</t>
         </is>
       </c>
     </row>
@@ -19082,12 +19082,12 @@
       <c r="AD184" t="inlineStr"/>
       <c r="AE184" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AF184" t="inlineStr">
         <is>
-          <t>administrativeInformation</t>
+          <t>modellingAndValidation/administrativeInformation</t>
         </is>
       </c>
     </row>
@@ -19172,12 +19172,12 @@
       <c r="AD185" t="inlineStr"/>
       <c r="AE185" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AF185" t="inlineStr">
         <is>
-          <t>commissionerAndGoal</t>
+          <t>modellingAndValidation/commissionerAndGoal</t>
         </is>
       </c>
     </row>
@@ -19294,12 +19294,12 @@
       <c r="AD186" t="inlineStr"/>
       <c r="AE186" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF186" t="inlineStr">
         <is>
-          <t>referenceToCommissioner</t>
+          <t>modellingAndValidation/commissionerAndGoal/referenceToCommissioner</t>
         </is>
       </c>
     </row>
@@ -19409,12 +19409,12 @@
       <c r="AD187" t="inlineStr"/>
       <c r="AE187" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF187" t="inlineStr">
         <is>
-          <t>project</t>
+          <t>modellingAndValidation/commissionerAndGoal/project</t>
         </is>
       </c>
     </row>
@@ -19511,12 +19511,12 @@
       <c r="AD188" t="inlineStr"/>
       <c r="AE188" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF188" t="inlineStr">
         <is>
-          <t>intendedApplications</t>
+          <t>modellingAndValidation/commissionerAndGoal/intendedApplications</t>
         </is>
       </c>
     </row>
@@ -19605,12 +19605,12 @@
       <c r="AD189" t="inlineStr"/>
       <c r="AE189" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF189" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>modellingAndValidation/commissionerAndGoal/other</t>
         </is>
       </c>
     </row>
@@ -19695,12 +19695,12 @@
       <c r="AD190" t="inlineStr"/>
       <c r="AE190" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AF190" t="inlineStr">
         <is>
-          <t>dataGenerator</t>
+          <t>modellingAndValidation/dataGenerator</t>
         </is>
       </c>
     </row>
@@ -19809,12 +19809,12 @@
       <c r="AD191" t="inlineStr"/>
       <c r="AE191" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF191" t="inlineStr">
         <is>
-          <t>referenceToPersonOrEntityGeneratingTheDataSet</t>
+          <t>modellingAndValidation/dataGenerator/referenceToPersonOrEntityGeneratingTheDataSet</t>
         </is>
       </c>
     </row>
@@ -19903,12 +19903,12 @@
       <c r="AD192" t="inlineStr"/>
       <c r="AE192" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF192" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>modellingAndValidation/dataGenerator/other</t>
         </is>
       </c>
     </row>
@@ -19997,12 +19997,12 @@
       <c r="AD193" t="inlineStr"/>
       <c r="AE193" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AF193" t="inlineStr">
         <is>
-          <t>dataEntryBy</t>
+          <t>modellingAndValidation/dataEntryBy</t>
         </is>
       </c>
     </row>
@@ -20108,12 +20108,12 @@
       <c r="AD194" t="inlineStr"/>
       <c r="AE194" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF194" t="inlineStr">
         <is>
-          <t>timeStamp</t>
+          <t>modellingAndValidation/dataEntryBy/timeStamp</t>
         </is>
       </c>
     </row>
@@ -20219,12 +20219,12 @@
       <c r="AD195" t="inlineStr"/>
       <c r="AE195" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF195" t="inlineStr">
         <is>
-          <t>referenceToDataSetFormat</t>
+          <t>modellingAndValidation/dataEntryBy/referenceToDataSetFormat</t>
         </is>
       </c>
     </row>
@@ -20313,12 +20313,12 @@
       <c r="AD196" t="inlineStr"/>
       <c r="AE196" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF196" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>modellingAndValidation/dataEntryBy/other</t>
         </is>
       </c>
     </row>
@@ -20407,12 +20407,12 @@
       <c r="AD197" t="inlineStr"/>
       <c r="AE197" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AF197" t="inlineStr">
         <is>
-          <t>publicationAndOwnership</t>
+          <t>modellingAndValidation/publicationAndOwnership</t>
         </is>
       </c>
     </row>
@@ -20517,12 +20517,12 @@
       <c r="AD198" t="inlineStr"/>
       <c r="AE198" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF198" t="inlineStr">
         <is>
-          <t>dataSetVersion</t>
+          <t>modellingAndValidation/publicationAndOwnership/dataSetVersion</t>
         </is>
       </c>
     </row>
@@ -20624,12 +20624,12 @@
       <c r="AD199" t="inlineStr"/>
       <c r="AE199" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF199" t="inlineStr">
         <is>
-          <t>referenceToPrecedingDataSetVersion</t>
+          <t>modellingAndValidation/publicationAndOwnership/referenceToPrecedingDataSetVersion</t>
         </is>
       </c>
     </row>
@@ -20722,12 +20722,12 @@
       <c r="AD200" t="inlineStr"/>
       <c r="AE200" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF200" t="inlineStr">
         <is>
-          <t>permanentDataSetURI</t>
+          <t>modellingAndValidation/publicationAndOwnership/permanentDataSetURI</t>
         </is>
       </c>
     </row>
@@ -20828,12 +20828,12 @@
       <c r="AD201" t="inlineStr"/>
       <c r="AE201" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF201" t="inlineStr">
         <is>
-          <t>dateOfLastRevision</t>
+          <t>modellingAndValidation/publicationAndOwnership/dateOfLastRevision</t>
         </is>
       </c>
     </row>
@@ -20946,12 +20946,12 @@
       <c r="AD202" t="inlineStr"/>
       <c r="AE202" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF202" t="inlineStr">
         <is>
-          <t>referenceToRegistrationAuthority</t>
+          <t>modellingAndValidation/publicationAndOwnership/referenceToRegistrationAuthority</t>
         </is>
       </c>
     </row>
@@ -21070,12 +21070,12 @@
       <c r="AD203" t="inlineStr"/>
       <c r="AE203" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF203" t="inlineStr">
         <is>
-          <t>registrationNumber</t>
+          <t>modellingAndValidation/publicationAndOwnership/registrationNumber</t>
         </is>
       </c>
     </row>
@@ -21180,12 +21180,12 @@
       <c r="AD204" t="inlineStr"/>
       <c r="AE204" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF204" t="inlineStr">
         <is>
-          <t>referenceToOwnershipOfDataSet</t>
+          <t>modellingAndValidation/publicationAndOwnership/referenceToOwnershipOfDataSet</t>
         </is>
       </c>
     </row>
@@ -21290,12 +21290,12 @@
       <c r="AD205" t="inlineStr"/>
       <c r="AE205" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF205" t="inlineStr">
         <is>
-          <t>copyright</t>
+          <t>modellingAndValidation/publicationAndOwnership/copyright</t>
         </is>
       </c>
     </row>
@@ -21405,12 +21405,12 @@
       <c r="AD206" t="inlineStr"/>
       <c r="AE206" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF206" t="inlineStr">
         <is>
-          <t>licenseType</t>
+          <t>modellingAndValidation/publicationAndOwnership/licenseType</t>
         </is>
       </c>
     </row>
@@ -21507,12 +21507,12 @@
       <c r="AD207" t="inlineStr"/>
       <c r="AE207" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF207" t="inlineStr">
         <is>
-          <t>accessRestrictions</t>
+          <t>modellingAndValidation/publicationAndOwnership/accessRestrictions</t>
         </is>
       </c>
     </row>
@@ -21601,12 +21601,12 @@
       <c r="AD208" t="inlineStr"/>
       <c r="AE208" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF208" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>modellingAndValidation/publicationAndOwnership/other</t>
         </is>
       </c>
     </row>
@@ -21719,12 +21719,12 @@
       <c r="AD209" t="inlineStr"/>
       <c r="AE209" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AF209" t="inlineStr">
         <is>
-          <t>referenceToPublisher</t>
+          <t>modellingAndValidation/publicationAndOwnership/other/referenceToPublisher</t>
         </is>
       </c>
     </row>
@@ -21915,12 +21915,12 @@
       <c r="AD211" t="inlineStr"/>
       <c r="AE211" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AF211" t="inlineStr">
         <is>
-          <t>exchange</t>
+          <t>exchanges/exchange</t>
         </is>
       </c>
     </row>
@@ -22013,12 +22013,12 @@
       <c r="AD212" t="inlineStr"/>
       <c r="AE212" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF212" t="inlineStr">
         <is>
-          <t>@dataSetInternalID</t>
+          <t>exchanges/exchange/@dataSetInternalID</t>
         </is>
       </c>
     </row>
@@ -22115,12 +22115,12 @@
       <c r="AD213" t="inlineStr"/>
       <c r="AE213" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF213" t="inlineStr">
         <is>
-          <t>referenceToFlowDataSet</t>
+          <t>exchanges/exchange/referenceToFlowDataSet</t>
         </is>
       </c>
     </row>
@@ -22210,12 +22210,12 @@
       <c r="AD214" t="inlineStr"/>
       <c r="AE214" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF214" t="inlineStr">
         <is>
-          <t>functionType</t>
+          <t>exchanges/exchange/functionType</t>
         </is>
       </c>
     </row>
@@ -22314,12 +22314,12 @@
       <c r="AD215" t="inlineStr"/>
       <c r="AE215" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF215" t="inlineStr">
         <is>
-          <t>exchangeDirection</t>
+          <t>exchanges/exchange/exchangeDirection</t>
         </is>
       </c>
     </row>
@@ -22416,12 +22416,12 @@
       <c r="AD216" t="inlineStr"/>
       <c r="AE216" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF216" t="inlineStr">
         <is>
-          <t>meanAmount</t>
+          <t>exchanges/exchange/meanAmount</t>
         </is>
       </c>
     </row>
@@ -22518,12 +22518,12 @@
       <c r="AD217" t="inlineStr"/>
       <c r="AE217" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF217" t="inlineStr">
         <is>
-          <t>generalComment</t>
+          <t>exchanges/exchange/generalComment</t>
         </is>
       </c>
     </row>
@@ -22612,12 +22612,12 @@
       <c r="AD218" t="inlineStr"/>
       <c r="AE218" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF218" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>exchanges/exchange/other</t>
         </is>
       </c>
     </row>
@@ -22796,12 +22796,12 @@
       <c r="AD220" t="inlineStr"/>
       <c r="AE220" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF220" t="inlineStr">
         <is>
-          <t>epd:amount</t>
+          <t>nan/epd:amount</t>
         </is>
       </c>
     </row>
@@ -22910,12 +22910,12 @@
       <c r="AD221" t="inlineStr"/>
       <c r="AE221" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF221" t="inlineStr">
         <is>
-          <t>@epd:module</t>
+          <t>nan/@epd:module</t>
         </is>
       </c>
     </row>
@@ -23004,12 +23004,12 @@
       <c r="AD222" t="inlineStr"/>
       <c r="AE222" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF222" t="inlineStr">
         <is>
-          <t>@epd:scenario</t>
+          <t>nan/@epd:scenario</t>
         </is>
       </c>
     </row>
@@ -23106,12 +23106,12 @@
       <c r="AD223" t="inlineStr"/>
       <c r="AE223" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF223" t="inlineStr">
         <is>
-          <t>epd:referenceToUnitGroupDataSet</t>
+          <t>nan/epd:referenceToUnitGroupDataSet</t>
         </is>
       </c>
     </row>
@@ -23290,12 +23290,12 @@
       <c r="AD225" t="inlineStr"/>
       <c r="AE225" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AF225" t="inlineStr">
         <is>
-          <t>LCIAResult</t>
+          <t>LCIAResults/LCIAResult</t>
         </is>
       </c>
     </row>
@@ -23396,12 +23396,12 @@
       <c r="AD226" t="inlineStr"/>
       <c r="AE226" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF226" t="inlineStr">
         <is>
-          <t>referenceToLCIAMethodDataSet</t>
+          <t>LCIAResults/LCIAResult/referenceToLCIAMethodDataSet</t>
         </is>
       </c>
     </row>
@@ -23498,12 +23498,12 @@
       <c r="AD227" t="inlineStr"/>
       <c r="AE227" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF227" t="inlineStr">
         <is>
-          <t>generalComment</t>
+          <t>LCIAResults/LCIAResult/generalComment</t>
         </is>
       </c>
     </row>
@@ -23592,12 +23592,12 @@
       <c r="AD228" t="inlineStr"/>
       <c r="AE228" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF228" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>LCIAResults/LCIAResult/other</t>
         </is>
       </c>
     </row>
@@ -23690,12 +23690,12 @@
       <c r="AD229" t="inlineStr"/>
       <c r="AE229" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF229" t="inlineStr">
         <is>
-          <t>epd:amount</t>
+          <t>LCIAResults/LCIAResult/epd:amount</t>
         </is>
       </c>
     </row>
@@ -23812,12 +23812,12 @@
       <c r="AD230" t="inlineStr"/>
       <c r="AE230" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF230" t="inlineStr">
         <is>
-          <t>@epd:module</t>
+          <t>LCIAResults/LCIAResult/@epd:module</t>
         </is>
       </c>
     </row>
@@ -23910,12 +23910,12 @@
       <c r="AD231" t="inlineStr"/>
       <c r="AE231" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF231" t="inlineStr">
         <is>
-          <t>@epd:scenario</t>
+          <t>LCIAResults/LCIAResult/@epd:scenario</t>
         </is>
       </c>
     </row>
@@ -24028,12 +24028,12 @@
       <c r="AD232" t="inlineStr"/>
       <c r="AE232" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF232" t="inlineStr">
         <is>
-          <t>epd:referenceToUnitGroupDataSet</t>
+          <t>LCIAResults/LCIAResult/epd:referenceToUnitGroupDataSet</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
intent taken from html and combined with xlsx
</commit_message>
<xml_diff>
--- a/output/roundtrip.xlsx
+++ b/output/roundtrip.xlsx
@@ -757,7 +757,7 @@
       <c r="AA3" t="inlineStr"/>
       <c r="AB3" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AC3" t="inlineStr">
@@ -844,7 +844,7 @@
       <c r="AA4" t="inlineStr"/>
       <c r="AB4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AC4" t="inlineStr">
@@ -1034,12 +1034,12 @@
       <c r="AA6" t="inlineStr"/>
       <c r="AB6" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AC6" t="inlineStr">
         <is>
-          <t>processDataSet/@locations/@metaDataOnly</t>
+          <t>processDataSet/@metaDataOnly</t>
         </is>
       </c>
     </row>
@@ -1125,12 +1125,12 @@
       <c r="AA7" t="inlineStr"/>
       <c r="AB7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AC7" t="inlineStr">
         <is>
-          <t>processInformation</t>
+          <t>processDataSet/processInformation</t>
         </is>
       </c>
     </row>
@@ -1216,12 +1216,12 @@
       <c r="AA8" t="inlineStr"/>
       <c r="AB8" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AC8" t="inlineStr">
         <is>
-          <t>processInformation/dataSetInformation</t>
+          <t>processDataSet/processInformation/dataSetInformation</t>
         </is>
       </c>
     </row>
@@ -1323,12 +1323,12 @@
       <c r="AA9" t="inlineStr"/>
       <c r="AB9" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC9" t="inlineStr">
         <is>
-          <t>processInformation/dataSetInformation/UUID</t>
+          <t>processDataSet/processInformation/dataSetInformation/UUID</t>
         </is>
       </c>
     </row>
@@ -1434,12 +1434,12 @@
       <c r="AA10" t="inlineStr"/>
       <c r="AB10" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC10" t="inlineStr">
         <is>
-          <t>processInformation/dataSetInformation/name</t>
+          <t>processDataSet/processInformation/dataSetInformation/name</t>
         </is>
       </c>
     </row>
@@ -1537,12 +1537,12 @@
       <c r="AA11" t="inlineStr"/>
       <c r="AB11" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="AC11" t="inlineStr">
         <is>
-          <t>processInformation/dataSetInformation/baseName</t>
+          <t>processDataSet/processInformation/dataSetInformation/name/baseName</t>
         </is>
       </c>
     </row>
@@ -1640,12 +1640,12 @@
       <c r="AA12" t="inlineStr"/>
       <c r="AB12" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="AC12" t="inlineStr">
         <is>
-          <t>processInformation/dataSetInformation/functionalUnitFlowProperties</t>
+          <t>processDataSet/processInformation/dataSetInformation/name/functionalUnitFlowProperties</t>
         </is>
       </c>
     </row>
@@ -1731,12 +1731,12 @@
       <c r="AA13" t="inlineStr"/>
       <c r="AB13" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC13" t="inlineStr">
         <is>
-          <t>processInformation/dataSetInformation/other</t>
+          <t>processDataSet/processInformation/dataSetInformation/other</t>
         </is>
       </c>
     </row>
@@ -1830,12 +1830,12 @@
       <c r="AA14" t="inlineStr"/>
       <c r="AB14" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC14" t="inlineStr">
         <is>
-          <t>processInformation/dataSetInformation/synonyms</t>
+          <t>processDataSet/processInformation/dataSetInformation/synonyms</t>
         </is>
       </c>
     </row>
@@ -1936,12 +1936,12 @@
       <c r="AA15" t="inlineStr"/>
       <c r="AB15" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC15" t="inlineStr">
         <is>
-          <t>processInformation/dataSetInformation/classificationInformation</t>
+          <t>processDataSet/processInformation/dataSetInformation/classificationInformation</t>
         </is>
       </c>
     </row>
@@ -2031,12 +2031,12 @@
       <c r="AA16" t="inlineStr"/>
       <c r="AB16" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="AC16" t="inlineStr">
         <is>
-          <t>processInformation/dataSetInformation/classification</t>
+          <t>processDataSet/processInformation/dataSetInformation/classificationInformation/classification</t>
         </is>
       </c>
     </row>
@@ -2126,12 +2126,12 @@
       <c r="AA17" t="inlineStr"/>
       <c r="AB17" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
       <c r="AC17" t="inlineStr">
         <is>
-          <t>processInformation/dataSetInformation/classification/@name</t>
+          <t>processDataSet/processInformation/dataSetInformation/classificationInformation/classification/@name</t>
         </is>
       </c>
     </row>
@@ -2221,12 +2221,12 @@
       <c r="AA18" t="inlineStr"/>
       <c r="AB18" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
       <c r="AC18" t="inlineStr">
         <is>
-          <t>processInformation/dataSetInformation/classification/@classes</t>
+          <t>processDataSet/processInformation/dataSetInformation/classificationInformation/classification/@classes</t>
         </is>
       </c>
     </row>
@@ -2316,12 +2316,12 @@
       <c r="AA19" t="inlineStr"/>
       <c r="AB19" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
       <c r="AC19" t="inlineStr">
         <is>
-          <t>processInformation/dataSetInformation/classification/class</t>
+          <t>processDataSet/processInformation/dataSetInformation/classificationInformation/classification/class</t>
         </is>
       </c>
     </row>
@@ -2411,12 +2411,12 @@
       <c r="AA20" t="inlineStr"/>
       <c r="AB20" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>6</t>
         </is>
       </c>
       <c r="AC20" t="inlineStr">
         <is>
-          <t>processInformation/dataSetInformation/classification/@level</t>
+          <t>processDataSet/processInformation/dataSetInformation/classificationInformation/classification/class/@level</t>
         </is>
       </c>
     </row>
@@ -2506,12 +2506,12 @@
       <c r="AA21" t="inlineStr"/>
       <c r="AB21" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>6</t>
         </is>
       </c>
       <c r="AC21" t="inlineStr">
         <is>
-          <t>processInformation/dataSetInformation/classification/@classId</t>
+          <t>processDataSet/processInformation/dataSetInformation/classificationInformation/classification/class/@classId</t>
         </is>
       </c>
     </row>
@@ -2625,12 +2625,12 @@
       <c r="AA22" t="inlineStr"/>
       <c r="AB22" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC22" t="inlineStr">
         <is>
-          <t>processInformation/dataSetInformation/generalComment</t>
+          <t>processDataSet/processInformation/dataSetInformation/generalComment</t>
         </is>
       </c>
     </row>
@@ -2742,12 +2742,12 @@
       <c r="AA23" t="inlineStr"/>
       <c r="AB23" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC23" t="inlineStr">
         <is>
-          <t>processInformation/dataSetInformation/referenceToExternalDocumentation</t>
+          <t>processDataSet/processInformation/dataSetInformation/referenceToExternalDocumentation</t>
         </is>
       </c>
     </row>
@@ -2833,12 +2833,12 @@
       <c r="AA24" t="inlineStr"/>
       <c r="AB24" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC24" t="inlineStr">
         <is>
-          <t>processInformation/dataSetInformation/other</t>
+          <t>processDataSet/processInformation/dataSetInformation/other</t>
         </is>
       </c>
     </row>
@@ -2920,12 +2920,12 @@
       <c r="AA25" t="inlineStr"/>
       <c r="AB25" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="AC25" t="inlineStr">
         <is>
-          <t>processInformation/epd24:referenceServiceLife</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd24:referenceServiceLife</t>
         </is>
       </c>
     </row>
@@ -3011,12 +3011,12 @@
       <c r="AA26" t="inlineStr"/>
       <c r="AB26" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="AC26" t="inlineStr">
         <is>
-          <t>processInformation/epd24:referenceServiceLife/@epd24:years</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd24:referenceServiceLife/@epd24:years</t>
         </is>
       </c>
     </row>
@@ -3098,12 +3098,12 @@
       <c r="AA27" t="inlineStr"/>
       <c r="AB27" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="AC27" t="inlineStr">
         <is>
-          <t>processInformation/epd24:referenceServiceLife/epd24:useConditionFactor</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd24:referenceServiceLife/epd24:useConditionFactor</t>
         </is>
       </c>
     </row>
@@ -3196,12 +3196,12 @@
       <c r="AA28" t="inlineStr"/>
       <c r="AB28" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>6</t>
         </is>
       </c>
       <c r="AC28" t="inlineStr">
         <is>
-          <t>processInformation/epd24:referenceServiceLife/@epd24:factorCategory</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd24:referenceServiceLife/epd24:useConditionFactor/@epd24:factorCategory</t>
         </is>
       </c>
     </row>
@@ -3293,12 +3293,12 @@
       <c r="AA29" t="inlineStr"/>
       <c r="AB29" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>6</t>
         </is>
       </c>
       <c r="AC29" t="inlineStr">
         <is>
-          <t>processInformation/epd24:referenceServiceLife/@epd24:objectSpecificGrade</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd24:referenceServiceLife/epd24:useConditionFactor/@epd24:objectSpecificGrade</t>
         </is>
       </c>
     </row>
@@ -3390,12 +3390,12 @@
       <c r="AA30" t="inlineStr"/>
       <c r="AB30" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>6</t>
         </is>
       </c>
       <c r="AC30" t="inlineStr">
         <is>
-          <t>processInformation/epd24:referenceServiceLife/@epd24:referenceGrade</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd24:referenceServiceLife/epd24:useConditionFactor/@epd24:referenceGrade</t>
         </is>
       </c>
     </row>
@@ -3481,12 +3481,12 @@
       <c r="AA31" t="inlineStr"/>
       <c r="AB31" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>6</t>
         </is>
       </c>
       <c r="AC31" t="inlineStr">
         <is>
-          <t>processInformation/epd24:referenceServiceLife/@epd24:factor</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd24:referenceServiceLife/epd24:useConditionFactor/@epd24:factor</t>
         </is>
       </c>
     </row>
@@ -3572,12 +3572,12 @@
       <c r="AA32" t="inlineStr"/>
       <c r="AB32" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="AC32" t="inlineStr">
         <is>
-          <t>processInformation/epd24:referenceServiceLife/epd24:comment</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd24:referenceServiceLife/epd24:comment</t>
         </is>
       </c>
     </row>
@@ -3663,12 +3663,12 @@
       <c r="AA33" t="inlineStr"/>
       <c r="AB33" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="AC33" t="inlineStr">
         <is>
-          <t>processInformation/epd24:referenceServiceLife/epd24:referenceToStandard</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd24:referenceServiceLife/epd24:referenceToStandard</t>
         </is>
       </c>
     </row>
@@ -3754,12 +3754,12 @@
       <c r="AA34" t="inlineStr"/>
       <c r="AB34" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="AC34" t="inlineStr">
         <is>
-          <t>processInformation/epd24:referenceServiceLife/epd24:referenceToUseConditionsDocumentation</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd24:referenceServiceLife/epd24:referenceToUseConditionsDocumentation</t>
         </is>
       </c>
     </row>
@@ -3845,12 +3845,12 @@
       <c r="AA35" t="inlineStr"/>
       <c r="AB35" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="AC35" t="inlineStr">
         <is>
-          <t>processInformation/epd24:referenceServiceLife/epd24:comment</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd24:referenceServiceLife/epd24:comment</t>
         </is>
       </c>
     </row>
@@ -3932,12 +3932,12 @@
       <c r="AA36" t="inlineStr"/>
       <c r="AB36" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="AC36" t="inlineStr">
         <is>
-          <t>processInformation/epd24:estimatedServiceLife</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd24:estimatedServiceLife</t>
         </is>
       </c>
     </row>
@@ -4023,12 +4023,12 @@
       <c r="AA37" t="inlineStr"/>
       <c r="AB37" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="AC37" t="inlineStr">
         <is>
-          <t>processInformation/epd24:estimatedServiceLife/@epd24:years</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd24:estimatedServiceLife/@epd24:years</t>
         </is>
       </c>
     </row>
@@ -4110,12 +4110,12 @@
       <c r="AA38" t="inlineStr"/>
       <c r="AB38" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="AC38" t="inlineStr">
         <is>
-          <t>processInformation/epd24:estimatedServiceLife/epd24:useConditionFactor</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd24:estimatedServiceLife/epd24:useConditionFactor</t>
         </is>
       </c>
     </row>
@@ -4208,12 +4208,12 @@
       <c r="AA39" t="inlineStr"/>
       <c r="AB39" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>6</t>
         </is>
       </c>
       <c r="AC39" t="inlineStr">
         <is>
-          <t>processInformation/epd24:estimatedServiceLife/@epd24:factorCategory</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd24:estimatedServiceLife/epd24:useConditionFactor/@epd24:factorCategory</t>
         </is>
       </c>
     </row>
@@ -4305,12 +4305,12 @@
       <c r="AA40" t="inlineStr"/>
       <c r="AB40" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>6</t>
         </is>
       </c>
       <c r="AC40" t="inlineStr">
         <is>
-          <t>processInformation/epd24:estimatedServiceLife/@epd24:objectSpecificGrade</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd24:estimatedServiceLife/epd24:useConditionFactor/@epd24:objectSpecificGrade</t>
         </is>
       </c>
     </row>
@@ -4402,12 +4402,12 @@
       <c r="AA41" t="inlineStr"/>
       <c r="AB41" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>6</t>
         </is>
       </c>
       <c r="AC41" t="inlineStr">
         <is>
-          <t>processInformation/epd24:estimatedServiceLife/@epd24:referenceGrade</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd24:estimatedServiceLife/epd24:useConditionFactor/@epd24:referenceGrade</t>
         </is>
       </c>
     </row>
@@ -4493,12 +4493,12 @@
       <c r="AA42" t="inlineStr"/>
       <c r="AB42" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>6</t>
         </is>
       </c>
       <c r="AC42" t="inlineStr">
         <is>
-          <t>processInformation/epd24:estimatedServiceLife/@epd24:factor</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd24:estimatedServiceLife/epd24:useConditionFactor/@epd24:factor</t>
         </is>
       </c>
     </row>
@@ -4584,12 +4584,12 @@
       <c r="AA43" t="inlineStr"/>
       <c r="AB43" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="AC43" t="inlineStr">
         <is>
-          <t>processInformation/epd24:estimatedServiceLife/epd24:comment</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd24:estimatedServiceLife/epd24:comment</t>
         </is>
       </c>
     </row>
@@ -4675,12 +4675,12 @@
       <c r="AA44" t="inlineStr"/>
       <c r="AB44" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="AC44" t="inlineStr">
         <is>
-          <t>processInformation/epd24:estimatedServiceLife/epd24:referenceToStandard</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd24:estimatedServiceLife/epd24:referenceToStandard</t>
         </is>
       </c>
     </row>
@@ -4766,12 +4766,12 @@
       <c r="AA45" t="inlineStr"/>
       <c r="AB45" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="AC45" t="inlineStr">
         <is>
-          <t>processInformation/epd24:estimatedServiceLife/epd24:referenceToUseConditionsDocumentation</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd24:estimatedServiceLife/epd24:referenceToUseConditionsDocumentation</t>
         </is>
       </c>
     </row>
@@ -4857,12 +4857,12 @@
       <c r="AA46" t="inlineStr"/>
       <c r="AB46" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="AC46" t="inlineStr">
         <is>
-          <t>processInformation/epd24:estimatedServiceLife/epd24:comment</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd24:estimatedServiceLife/epd24:comment</t>
         </is>
       </c>
     </row>
@@ -4940,12 +4940,12 @@
       <c r="AA47" t="inlineStr"/>
       <c r="AB47" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="AC47" t="inlineStr">
         <is>
-          <t>processInformation/epd24:productIds</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd24:productIds</t>
         </is>
       </c>
     </row>
@@ -5031,12 +5031,12 @@
       <c r="AA48" t="inlineStr"/>
       <c r="AB48" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="AC48" t="inlineStr">
         <is>
-          <t>processInformation/epd24:productIds/epd24:productId</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd24:productIds/epd24:productId</t>
         </is>
       </c>
     </row>
@@ -5122,12 +5122,12 @@
       <c r="AA49" t="inlineStr"/>
       <c r="AB49" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>6</t>
         </is>
       </c>
       <c r="AC49" t="inlineStr">
         <is>
-          <t>processInformation/epd24:productIds/@epd24:type</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd24:productIds/epd24:productId/@epd24:type</t>
         </is>
       </c>
     </row>
@@ -5226,12 +5226,12 @@
       <c r="AA50" t="inlineStr"/>
       <c r="AB50" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="AC50" t="inlineStr">
         <is>
-          <t>processInformation/epd:safetyMargins</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd:safetyMargins</t>
         </is>
       </c>
     </row>
@@ -5321,12 +5321,12 @@
       <c r="AA51" t="inlineStr"/>
       <c r="AB51" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="AC51" t="inlineStr">
         <is>
-          <t>processInformation/epd:safetyMargins/epd:margins</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd:safetyMargins/epd:margins</t>
         </is>
       </c>
     </row>
@@ -5429,12 +5429,12 @@
       <c r="AA52" t="inlineStr"/>
       <c r="AB52" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>6</t>
         </is>
       </c>
       <c r="AC52" t="inlineStr">
         <is>
-          <t>processInformation/epd:safetyMargins/epd:description</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd:safetyMargins/epd:margins/epd:description</t>
         </is>
       </c>
     </row>
@@ -5530,12 +5530,12 @@
       <c r="AA53" t="inlineStr"/>
       <c r="AB53" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="AC53" t="inlineStr">
         <is>
-          <t>processInformation/epd:scenarios</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd:scenarios</t>
         </is>
       </c>
     </row>
@@ -5633,12 +5633,12 @@
       <c r="AA54" t="inlineStr"/>
       <c r="AB54" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="AC54" t="inlineStr">
         <is>
-          <t>processInformation/epd:scenarios/epd:scenario</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd:scenarios/epd:scenario</t>
         </is>
       </c>
     </row>
@@ -5736,12 +5736,12 @@
       <c r="AA55" t="inlineStr"/>
       <c r="AB55" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>6</t>
         </is>
       </c>
       <c r="AC55" t="inlineStr">
         <is>
-          <t>processInformation/epd:scenarios/@epd:name</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd:scenarios/epd:scenario/@epd:name</t>
         </is>
       </c>
     </row>
@@ -5827,12 +5827,12 @@
       <c r="AA56" t="inlineStr"/>
       <c r="AB56" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>6</t>
         </is>
       </c>
       <c r="AC56" t="inlineStr">
         <is>
-          <t>processInformation/epd:scenarios/@epd:default</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd:scenarios/epd:scenario/@epd:default</t>
         </is>
       </c>
     </row>
@@ -5918,12 +5918,12 @@
       <c r="AA57" t="inlineStr"/>
       <c r="AB57" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>6</t>
         </is>
       </c>
       <c r="AC57" t="inlineStr">
         <is>
-          <t>processInformation/epd:scenarios/@epd:group</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd:scenarios/epd:scenario/@epd:group</t>
         </is>
       </c>
     </row>
@@ -6025,12 +6025,12 @@
       <c r="AA58" t="inlineStr"/>
       <c r="AB58" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>6</t>
         </is>
       </c>
       <c r="AC58" t="inlineStr">
         <is>
-          <t>processInformation/epd:scenarios/epd:description</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd:scenarios/epd:scenario/epd:description</t>
         </is>
       </c>
     </row>
@@ -6112,12 +6112,12 @@
       <c r="AA59" t="inlineStr"/>
       <c r="AB59" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="AC59" t="inlineStr">
         <is>
-          <t>processInformation/epd:modules</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd:modules</t>
         </is>
       </c>
     </row>
@@ -6203,12 +6203,12 @@
       <c r="AA60" t="inlineStr"/>
       <c r="AB60" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="AC60" t="inlineStr">
         <is>
-          <t>processInformation/epd:modules/epd:module</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd:modules/epd:module</t>
         </is>
       </c>
     </row>
@@ -6294,12 +6294,12 @@
       <c r="AA61" t="inlineStr"/>
       <c r="AB61" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>6</t>
         </is>
       </c>
       <c r="AC61" t="inlineStr">
         <is>
-          <t>processInformation/epd:modules/@epd:name</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd:modules/epd:module/@epd:name</t>
         </is>
       </c>
     </row>
@@ -6385,12 +6385,12 @@
       <c r="AA62" t="inlineStr"/>
       <c r="AB62" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>6</t>
         </is>
       </c>
       <c r="AC62" t="inlineStr">
         <is>
-          <t>processInformation/epd:modules/@epd:productsystem-id</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd:modules/epd:module/@epd:productsystem-id</t>
         </is>
       </c>
     </row>
@@ -6499,12 +6499,12 @@
       <c r="AA63" t="inlineStr"/>
       <c r="AB63" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="AC63" t="inlineStr">
         <is>
-          <t>processInformation/epd2:contentDeclaration</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd2:contentDeclaration</t>
         </is>
       </c>
     </row>
@@ -6586,12 +6586,12 @@
       <c r="AA64" t="inlineStr"/>
       <c r="AB64" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="AC64" t="inlineStr">
         <is>
-          <t>processInformation/epd2:contentDeclaration/epd2:component</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd2:contentDeclaration/epd2:component</t>
         </is>
       </c>
     </row>
@@ -6677,12 +6677,12 @@
       <c r="AA65" t="inlineStr"/>
       <c r="AB65" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>6</t>
         </is>
       </c>
       <c r="AC65" t="inlineStr">
         <is>
-          <t>processInformation/epd2:contentDeclaration/epd2:name</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd2:contentDeclaration/epd2:component/epd2:name</t>
         </is>
       </c>
     </row>
@@ -6764,12 +6764,12 @@
       <c r="AA66" t="inlineStr"/>
       <c r="AB66" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>7</t>
         </is>
       </c>
       <c r="AC66" t="inlineStr">
         <is>
-          <t>processInformation/epd2:contentDeclaration/epd2:weightPerc</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd2:contentDeclaration/epd2:component/epd2:name/epd2:weightPerc</t>
         </is>
       </c>
     </row>
@@ -6851,12 +6851,12 @@
       <c r="AA67" t="inlineStr"/>
       <c r="AB67" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>8</t>
         </is>
       </c>
       <c r="AC67" t="inlineStr">
         <is>
-          <t>processInformation/epd2:contentDeclaration/@epd2:value</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd2:contentDeclaration/epd2:component/epd2:name/epd2:weightPerc/@epd2:value</t>
         </is>
       </c>
     </row>
@@ -6938,12 +6938,12 @@
       <c r="AA68" t="inlineStr"/>
       <c r="AB68" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>8</t>
         </is>
       </c>
       <c r="AC68" t="inlineStr">
         <is>
-          <t>processInformation/epd2:contentDeclaration/@epd2:lowerValue</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd2:contentDeclaration/epd2:component/epd2:name/epd2:weightPerc/@epd2:lowerValue</t>
         </is>
       </c>
     </row>
@@ -7025,12 +7025,12 @@
       <c r="AA69" t="inlineStr"/>
       <c r="AB69" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>8</t>
         </is>
       </c>
       <c r="AC69" t="inlineStr">
         <is>
-          <t>processInformation/epd2:contentDeclaration/@epd2:upperValue</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd2:contentDeclaration/epd2:component/epd2:name/epd2:weightPerc/@epd2:upperValue</t>
         </is>
       </c>
     </row>
@@ -7112,12 +7112,12 @@
       <c r="AA70" t="inlineStr"/>
       <c r="AB70" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>7</t>
         </is>
       </c>
       <c r="AC70" t="inlineStr">
         <is>
-          <t>processInformation/epd2:contentDeclaration/epd2:mass</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd2:contentDeclaration/epd2:component/epd2:name/epd2:mass</t>
         </is>
       </c>
     </row>
@@ -7199,12 +7199,12 @@
       <c r="AA71" t="inlineStr"/>
       <c r="AB71" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>8</t>
         </is>
       </c>
       <c r="AC71" t="inlineStr">
         <is>
-          <t>processInformation/epd2:contentDeclaration/@epd2:value</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd2:contentDeclaration/epd2:component/epd2:name/epd2:mass/@epd2:value</t>
         </is>
       </c>
     </row>
@@ -7286,12 +7286,12 @@
       <c r="AA72" t="inlineStr"/>
       <c r="AB72" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>8</t>
         </is>
       </c>
       <c r="AC72" t="inlineStr">
         <is>
-          <t>processInformation/epd2:contentDeclaration/@epd2:lowerValue</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd2:contentDeclaration/epd2:component/epd2:name/epd2:mass/@epd2:lowerValue</t>
         </is>
       </c>
     </row>
@@ -7373,12 +7373,12 @@
       <c r="AA73" t="inlineStr"/>
       <c r="AB73" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>8</t>
         </is>
       </c>
       <c r="AC73" t="inlineStr">
         <is>
-          <t>processInformation/epd2:contentDeclaration/@epd2:upperValue</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd2:contentDeclaration/epd2:component/epd2:name/epd2:mass/@epd2:upperValue</t>
         </is>
       </c>
     </row>
@@ -7464,12 +7464,12 @@
       <c r="AA74" t="inlineStr"/>
       <c r="AB74" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>7</t>
         </is>
       </c>
       <c r="AC74" t="inlineStr">
         <is>
-          <t>processInformation/epd2:contentDeclaration/epd2:comment</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd2:contentDeclaration/epd2:component/epd2:name/epd2:comment</t>
         </is>
       </c>
     </row>
@@ -7551,12 +7551,12 @@
       <c r="AA75" t="inlineStr"/>
       <c r="AB75" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>6</t>
         </is>
       </c>
       <c r="AC75" t="inlineStr">
         <is>
-          <t>processInformation/epd2:contentDeclaration/epd2:material_|_epd2:substance</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd2:contentDeclaration/epd2:component/epd2:material_|_epd2:substance</t>
         </is>
       </c>
     </row>
@@ -7642,12 +7642,12 @@
       <c r="AA76" t="inlineStr"/>
       <c r="AB76" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>6</t>
         </is>
       </c>
       <c r="AC76" t="inlineStr">
         <is>
-          <t>processInformation/epd2:contentDeclaration/epd2:name</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd2:contentDeclaration/epd2:component/epd2:name</t>
         </is>
       </c>
     </row>
@@ -7729,12 +7729,12 @@
       <c r="AA77" t="inlineStr"/>
       <c r="AB77" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>7</t>
         </is>
       </c>
       <c r="AC77" t="inlineStr">
         <is>
-          <t>processInformation/epd2:contentDeclaration/epd2:weightPerc</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd2:contentDeclaration/epd2:component/epd2:name/epd2:weightPerc</t>
         </is>
       </c>
     </row>
@@ -7816,12 +7816,12 @@
       <c r="AA78" t="inlineStr"/>
       <c r="AB78" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>8</t>
         </is>
       </c>
       <c r="AC78" t="inlineStr">
         <is>
-          <t>processInformation/epd2:contentDeclaration/@epd2:value</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd2:contentDeclaration/epd2:component/epd2:name/epd2:weightPerc/@epd2:value</t>
         </is>
       </c>
     </row>
@@ -7903,12 +7903,12 @@
       <c r="AA79" t="inlineStr"/>
       <c r="AB79" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>8</t>
         </is>
       </c>
       <c r="AC79" t="inlineStr">
         <is>
-          <t>processInformation/epd2:contentDeclaration/@epd2:lowerValue</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd2:contentDeclaration/epd2:component/epd2:name/epd2:weightPerc/@epd2:lowerValue</t>
         </is>
       </c>
     </row>
@@ -7990,12 +7990,12 @@
       <c r="AA80" t="inlineStr"/>
       <c r="AB80" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>8</t>
         </is>
       </c>
       <c r="AC80" t="inlineStr">
         <is>
-          <t>processInformation/epd2:contentDeclaration/@epd2:upperValue</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd2:contentDeclaration/epd2:component/epd2:name/epd2:weightPerc/@epd2:upperValue</t>
         </is>
       </c>
     </row>
@@ -8077,12 +8077,12 @@
       <c r="AA81" t="inlineStr"/>
       <c r="AB81" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>7</t>
         </is>
       </c>
       <c r="AC81" t="inlineStr">
         <is>
-          <t>processInformation/epd2:contentDeclaration/epd2:mass</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd2:contentDeclaration/epd2:component/epd2:name/epd2:mass</t>
         </is>
       </c>
     </row>
@@ -8164,12 +8164,12 @@
       <c r="AA82" t="inlineStr"/>
       <c r="AB82" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>8</t>
         </is>
       </c>
       <c r="AC82" t="inlineStr">
         <is>
-          <t>processInformation/epd2:contentDeclaration/@epd2:value</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd2:contentDeclaration/epd2:component/epd2:name/epd2:mass/@epd2:value</t>
         </is>
       </c>
     </row>
@@ -8251,12 +8251,12 @@
       <c r="AA83" t="inlineStr"/>
       <c r="AB83" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>8</t>
         </is>
       </c>
       <c r="AC83" t="inlineStr">
         <is>
-          <t>processInformation/epd2:contentDeclaration/@epd2:lowerValue</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd2:contentDeclaration/epd2:component/epd2:name/epd2:mass/@epd2:lowerValue</t>
         </is>
       </c>
     </row>
@@ -8338,12 +8338,12 @@
       <c r="AA84" t="inlineStr"/>
       <c r="AB84" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>8</t>
         </is>
       </c>
       <c r="AC84" t="inlineStr">
         <is>
-          <t>processInformation/epd2:contentDeclaration/@epd2:upperValue</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd2:contentDeclaration/epd2:component/epd2:name/epd2:mass/@epd2:upperValue</t>
         </is>
       </c>
     </row>
@@ -8425,12 +8425,12 @@
       <c r="AA85" t="inlineStr"/>
       <c r="AB85" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>7</t>
         </is>
       </c>
       <c r="AC85" t="inlineStr">
         <is>
-          <t>processInformation/epd2:contentDeclaration/@epd2:CASNumber</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd2:contentDeclaration/epd2:component/epd2:name/@epd2:CASNumber</t>
         </is>
       </c>
     </row>
@@ -8512,12 +8512,12 @@
       <c r="AA86" t="inlineStr"/>
       <c r="AB86" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>7</t>
         </is>
       </c>
       <c r="AC86" t="inlineStr">
         <is>
-          <t>processInformation/epd2:contentDeclaration/@epd2:ECNumber</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd2:contentDeclaration/epd2:component/epd2:name/@epd2:ECNumber</t>
         </is>
       </c>
     </row>
@@ -8599,12 +8599,12 @@
       <c r="AA87" t="inlineStr"/>
       <c r="AB87" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>7</t>
         </is>
       </c>
       <c r="AC87" t="inlineStr">
         <is>
-          <t>processInformation/epd2:contentDeclaration/@epd2:hazardCode</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd2:contentDeclaration/epd2:component/epd2:name/@epd2:hazardCode</t>
         </is>
       </c>
     </row>
@@ -8686,12 +8686,12 @@
       <c r="AA88" t="inlineStr"/>
       <c r="AB88" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>7</t>
         </is>
       </c>
       <c r="AC88" t="inlineStr">
         <is>
-          <t>processInformation/epd2:contentDeclaration/@epd2:renewable</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd2:contentDeclaration/epd2:component/epd2:name/@epd2:renewable</t>
         </is>
       </c>
     </row>
@@ -8773,12 +8773,12 @@
       <c r="AA89" t="inlineStr"/>
       <c r="AB89" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>7</t>
         </is>
       </c>
       <c r="AC89" t="inlineStr">
         <is>
-          <t>processInformation/epd2:contentDeclaration/@epd2:recycled</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd2:contentDeclaration/epd2:component/epd2:name/@epd2:recycled</t>
         </is>
       </c>
     </row>
@@ -8860,12 +8860,12 @@
       <c r="AA90" t="inlineStr"/>
       <c r="AB90" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>7</t>
         </is>
       </c>
       <c r="AC90" t="inlineStr">
         <is>
-          <t>processInformation/epd2:contentDeclaration/@epd2:recyclable</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd2:contentDeclaration/epd2:component/epd2:name/@epd2:recyclable</t>
         </is>
       </c>
     </row>
@@ -8947,12 +8947,12 @@
       <c r="AA91" t="inlineStr"/>
       <c r="AB91" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>7</t>
         </is>
       </c>
       <c r="AC91" t="inlineStr">
         <is>
-          <t>processInformation/epd2:contentDeclaration/@epd2:packaging</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd2:contentDeclaration/epd2:component/epd2:name/@epd2:packaging</t>
         </is>
       </c>
     </row>
@@ -9034,12 +9034,12 @@
       <c r="AA92" t="inlineStr"/>
       <c r="AB92" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>7</t>
         </is>
       </c>
       <c r="AC92" t="inlineStr">
         <is>
-          <t>processInformation/epd2:contentDeclaration/epd2:comment</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd2:contentDeclaration/epd2:component/epd2:name/epd2:comment</t>
         </is>
       </c>
     </row>
@@ -9125,12 +9125,12 @@
       <c r="AA93" t="inlineStr"/>
       <c r="AB93" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="AC93" t="inlineStr">
         <is>
-          <t>processInformation/epd2:contentDeclaration/epd24:SVHC</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd24:SVHC</t>
         </is>
       </c>
     </row>
@@ -9212,12 +9212,12 @@
       <c r="AA94" t="inlineStr"/>
       <c r="AB94" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="AC94" t="inlineStr">
         <is>
-          <t>processInformation/epd24:scenarioData</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd24:scenarioData</t>
         </is>
       </c>
     </row>
@@ -9299,12 +9299,12 @@
       <c r="AA95" t="inlineStr"/>
       <c r="AB95" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="AC95" t="inlineStr">
         <is>
-          <t>processInformation/epd24:scenarioData/epd24:useStageScenarioData</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd24:scenarioData/epd24:useStageScenarioData</t>
         </is>
       </c>
     </row>
@@ -9390,12 +9390,12 @@
       <c r="AA96" t="inlineStr"/>
       <c r="AB96" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>6</t>
         </is>
       </c>
       <c r="AC96" t="inlineStr">
         <is>
-          <t>processInformation/epd24:scenarioData/@epd24:scenario</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd24:scenarioData/epd24:useStageScenarioData/@epd24:scenario</t>
         </is>
       </c>
     </row>
@@ -9485,12 +9485,12 @@
       <c r="AA97" t="inlineStr"/>
       <c r="AB97" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>6</t>
         </is>
       </c>
       <c r="AC97" t="inlineStr">
         <is>
-          <t>processInformation/epd24:soilAndWaterImpacts</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd24:scenarioData/epd24:useStageScenarioData/epd24:soilAndWaterImpacts</t>
         </is>
       </c>
     </row>
@@ -9576,12 +9576,12 @@
       <c r="AA98" t="inlineStr"/>
       <c r="AB98" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>7</t>
         </is>
       </c>
       <c r="AC98" t="inlineStr">
         <is>
-          <t>processInformation/epd24:soilAndWaterImpacts/epd24:soilAndWaterImpactsDescription</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd24:scenarioData/epd24:useStageScenarioData/epd24:soilAndWaterImpacts/epd24:soilAndWaterImpactsDescription</t>
         </is>
       </c>
     </row>
@@ -9676,12 +9676,12 @@
       <c r="AA99" t="inlineStr"/>
       <c r="AB99" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="AC99" t="inlineStr">
         <is>
-          <t>processInformation/epd24:eolScenarioData</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd24:scenarioData/epd24:eolScenarioData</t>
         </is>
       </c>
     </row>
@@ -9767,12 +9767,12 @@
       <c r="AA100" t="inlineStr"/>
       <c r="AB100" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>6</t>
         </is>
       </c>
       <c r="AC100" t="inlineStr">
         <is>
-          <t>processInformation/epd24:eolScenarioData/@epd24:scenario</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd24:scenarioData/epd24:eolScenarioData/@epd24:scenario</t>
         </is>
       </c>
     </row>
@@ -9854,12 +9854,12 @@
       <c r="AA101" t="inlineStr"/>
       <c r="AB101" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>6</t>
         </is>
       </c>
       <c r="AC101" t="inlineStr">
         <is>
-          <t>processInformation/epd24:eolScenarioData/epd24:collection</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd24:scenarioData/epd24:eolScenarioData/epd24:collection</t>
         </is>
       </c>
     </row>
@@ -9945,12 +9945,12 @@
       <c r="AA102" t="inlineStr"/>
       <c r="AB102" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>7</t>
         </is>
       </c>
       <c r="AC102" t="inlineStr">
         <is>
-          <t>processInformation/epd24:eolScenarioData/@epd24:separate</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd24:scenarioData/epd24:eolScenarioData/epd24:collection/@epd24:separate</t>
         </is>
       </c>
     </row>
@@ -10036,12 +10036,12 @@
       <c r="AA103" t="inlineStr"/>
       <c r="AB103" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>7</t>
         </is>
       </c>
       <c r="AC103" t="inlineStr">
         <is>
-          <t>processInformation/epd24:eolScenarioData/@epd24:withMixedWaste</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd24:scenarioData/epd24:eolScenarioData/epd24:collection/@epd24:withMixedWaste</t>
         </is>
       </c>
     </row>
@@ -10123,12 +10123,12 @@
       <c r="AA104" t="inlineStr"/>
       <c r="AB104" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>6</t>
         </is>
       </c>
       <c r="AC104" t="inlineStr">
         <is>
-          <t>processInformation/epd24:eolScenarioData/epd24:recovery</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd24:scenarioData/epd24:eolScenarioData/epd24:recovery</t>
         </is>
       </c>
     </row>
@@ -10214,12 +10214,12 @@
       <c r="AA105" t="inlineStr"/>
       <c r="AB105" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>7</t>
         </is>
       </c>
       <c r="AC105" t="inlineStr">
         <is>
-          <t>processInformation/epd24:eolScenarioData/@epd24:reuse</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd24:scenarioData/epd24:eolScenarioData/epd24:recovery/@epd24:reuse</t>
         </is>
       </c>
     </row>
@@ -10305,12 +10305,12 @@
       <c r="AA106" t="inlineStr"/>
       <c r="AB106" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>7</t>
         </is>
       </c>
       <c r="AC106" t="inlineStr">
         <is>
-          <t>processInformation/epd24:eolScenarioData/@epd24:recycling</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd24:scenarioData/epd24:eolScenarioData/epd24:recovery/@epd24:recycling</t>
         </is>
       </c>
     </row>
@@ -10396,12 +10396,12 @@
       <c r="AA107" t="inlineStr"/>
       <c r="AB107" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>7</t>
         </is>
       </c>
       <c r="AC107" t="inlineStr">
         <is>
-          <t>processInformation/epd24:eolScenarioData/@epd24:energyRecovery</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd24:scenarioData/epd24:eolScenarioData/epd24:recovery/@epd24:energyRecovery</t>
         </is>
       </c>
     </row>
@@ -10483,12 +10483,12 @@
       <c r="AA108" t="inlineStr"/>
       <c r="AB108" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>6</t>
         </is>
       </c>
       <c r="AC108" t="inlineStr">
         <is>
-          <t>processInformation/epd24:eolScenarioData/epd24:disposal</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd24:scenarioData/epd24:eolScenarioData/epd24:disposal</t>
         </is>
       </c>
     </row>
@@ -10574,12 +10574,12 @@
       <c r="AA109" t="inlineStr"/>
       <c r="AB109" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>7</t>
         </is>
       </c>
       <c r="AC109" t="inlineStr">
         <is>
-          <t>processInformation/epd24:eolScenarioData/@epd24:finalDeposition</t>
+          <t>processDataSet/processInformation/dataSetInformation/other/epd24:scenarioData/epd24:eolScenarioData/epd24:disposal/@epd24:finalDeposition</t>
         </is>
       </c>
     </row>
@@ -10661,12 +10661,12 @@
       <c r="AA110" t="inlineStr"/>
       <c r="AB110" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AC110" t="inlineStr">
         <is>
-          <t>processInformation/quantitativeReference</t>
+          <t>processDataSet/processInformation/quantitativeReference</t>
         </is>
       </c>
     </row>
@@ -10760,12 +10760,12 @@
       <c r="AA111" t="inlineStr"/>
       <c r="AB111" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="AC111" t="inlineStr">
         <is>
-          <t>processInformation/quantitativeReference/@type</t>
+          <t>processDataSet/processInformation/quantitativeReference/@type</t>
         </is>
       </c>
     </row>
@@ -10879,12 +10879,12 @@
       <c r="AA112" t="inlineStr"/>
       <c r="AB112" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC112" t="inlineStr">
         <is>
-          <t>processInformation/quantitativeReference/referenceToReferenceFlow</t>
+          <t>processDataSet/processInformation/quantitativeReference/referenceToReferenceFlow</t>
         </is>
       </c>
     </row>
@@ -10986,12 +10986,12 @@
       <c r="AA113" t="inlineStr"/>
       <c r="AB113" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC113" t="inlineStr">
         <is>
-          <t>processInformation/quantitativeReference/functionalUnitOrOther</t>
+          <t>processDataSet/processInformation/quantitativeReference/functionalUnitOrOther</t>
         </is>
       </c>
     </row>
@@ -11077,12 +11077,12 @@
       <c r="AA114" t="inlineStr"/>
       <c r="AB114" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC114" t="inlineStr">
         <is>
-          <t>processInformation/quantitativeReference/other</t>
+          <t>processDataSet/processInformation/quantitativeReference/other</t>
         </is>
       </c>
     </row>
@@ -11164,12 +11164,12 @@
       <c r="AA115" t="inlineStr"/>
       <c r="AB115" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AC115" t="inlineStr">
         <is>
-          <t>processInformation/time</t>
+          <t>processDataSet/processInformation/time</t>
         </is>
       </c>
     </row>
@@ -11271,12 +11271,12 @@
       <c r="AA116" t="inlineStr"/>
       <c r="AB116" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC116" t="inlineStr">
         <is>
-          <t>processInformation/time/referenceYear</t>
+          <t>processDataSet/processInformation/time/referenceYear</t>
         </is>
       </c>
     </row>
@@ -11382,12 +11382,12 @@
       <c r="AA117" t="inlineStr"/>
       <c r="AB117" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC117" t="inlineStr">
         <is>
-          <t>processInformation/time/dataSetValidUntil</t>
+          <t>processDataSet/processInformation/time/dataSetValidUntil</t>
         </is>
       </c>
     </row>
@@ -11485,12 +11485,12 @@
       <c r="AA118" t="inlineStr"/>
       <c r="AB118" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC118" t="inlineStr">
         <is>
-          <t>processInformation/time/timeRepresentativenessDescription</t>
+          <t>processDataSet/processInformation/time/timeRepresentativenessDescription</t>
         </is>
       </c>
     </row>
@@ -11576,12 +11576,12 @@
       <c r="AA119" t="inlineStr"/>
       <c r="AB119" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC119" t="inlineStr">
         <is>
-          <t>processInformation/time/other</t>
+          <t>processDataSet/processInformation/time/other</t>
         </is>
       </c>
     </row>
@@ -11687,12 +11687,12 @@
       <c r="AA120" t="inlineStr"/>
       <c r="AB120" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="AC120" t="inlineStr">
         <is>
-          <t>processInformation/time/other/epd2:publicationDateOfEPD</t>
+          <t>processDataSet/processInformation/time/other/epd2:publicationDateOfEPD</t>
         </is>
       </c>
     </row>
@@ -11778,12 +11778,12 @@
       <c r="AA121" t="inlineStr"/>
       <c r="AB121" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="AC121" t="inlineStr">
         <is>
-          <t>processInformation/time/epd2:expirationDateOfEPD</t>
+          <t>processDataSet/processInformation/time/other/epd2:expirationDateOfEPD</t>
         </is>
       </c>
     </row>
@@ -11869,12 +11869,12 @@
       <c r="AA122" t="inlineStr"/>
       <c r="AB122" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AC122" t="inlineStr">
         <is>
-          <t>processInformation/geography</t>
+          <t>processDataSet/processInformation/geography</t>
         </is>
       </c>
     </row>
@@ -11960,12 +11960,12 @@
       <c r="AA123" t="inlineStr"/>
       <c r="AB123" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC123" t="inlineStr">
         <is>
-          <t>processInformation/geography/locationOfOperationSupplyOrProduction</t>
+          <t>processDataSet/processInformation/geography/locationOfOperationSupplyOrProduction</t>
         </is>
       </c>
     </row>
@@ -12071,12 +12071,12 @@
       <c r="AA124" t="inlineStr"/>
       <c r="AB124" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="AC124" t="inlineStr">
         <is>
-          <t>processInformation/geography/@location</t>
+          <t>processDataSet/processInformation/geography/locationOfOperationSupplyOrProduction/@location</t>
         </is>
       </c>
     </row>
@@ -12183,12 +12183,12 @@
       <c r="AA125" t="inlineStr"/>
       <c r="AB125" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="AC125" t="inlineStr">
         <is>
-          <t>processInformation/geography/descriptionOfRestrictions</t>
+          <t>processDataSet/processInformation/geography/locationOfOperationSupplyOrProduction/descriptionOfRestrictions</t>
         </is>
       </c>
     </row>
@@ -12274,12 +12274,12 @@
       <c r="AA126" t="inlineStr"/>
       <c r="AB126" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC126" t="inlineStr">
         <is>
-          <t>processInformation/geography/other</t>
+          <t>processDataSet/processInformation/geography/other</t>
         </is>
       </c>
     </row>
@@ -12365,12 +12365,12 @@
       <c r="AA127" t="inlineStr"/>
       <c r="AB127" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AC127" t="inlineStr">
         <is>
-          <t>processInformation/technology</t>
+          <t>processDataSet/processInformation/technology</t>
         </is>
       </c>
     </row>
@@ -12504,12 +12504,12 @@
       <c r="AA128" t="inlineStr"/>
       <c r="AB128" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC128" t="inlineStr">
         <is>
-          <t>processInformation/technology/technologyDescriptionAndIncludedProcesses</t>
+          <t>processDataSet/processInformation/technology/technologyDescriptionAndIncludedProcesses</t>
         </is>
       </c>
     </row>
@@ -12636,12 +12636,12 @@
       <c r="AA129" t="inlineStr"/>
       <c r="AB129" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC129" t="inlineStr">
         <is>
-          <t>processInformation/technology/technologicalApplicability</t>
+          <t>processDataSet/processInformation/technology/technologicalApplicability</t>
         </is>
       </c>
     </row>
@@ -12740,12 +12740,12 @@
       <c r="AA130" t="inlineStr"/>
       <c r="AB130" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC130" t="inlineStr">
         <is>
-          <t>processInformation/technology/referenceToTechnologyPictogramme</t>
+          <t>processDataSet/processInformation/technology/referenceToTechnologyPictogramme</t>
         </is>
       </c>
     </row>
@@ -12858,12 +12858,12 @@
       <c r="AA131" t="inlineStr"/>
       <c r="AB131" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC131" t="inlineStr">
         <is>
-          <t>processInformation/technology/referenceToTechnologyFlowDiagrammOrPicture</t>
+          <t>processDataSet/processInformation/technology/referenceToTechnologyFlowDiagrammOrPicture</t>
         </is>
       </c>
     </row>
@@ -12949,12 +12949,12 @@
       <c r="AA132" t="inlineStr"/>
       <c r="AB132" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC132" t="inlineStr">
         <is>
-          <t>processInformation/technology/other</t>
+          <t>processDataSet/processInformation/technology/other</t>
         </is>
       </c>
     </row>
@@ -13040,12 +13040,12 @@
       <c r="AA133" t="inlineStr"/>
       <c r="AB133" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AC133" t="inlineStr">
         <is>
-          <t>modellingAndValidation</t>
+          <t>processDataSet/modellingAndValidation</t>
         </is>
       </c>
     </row>
@@ -13131,12 +13131,12 @@
       <c r="AA134" t="inlineStr"/>
       <c r="AB134" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AC134" t="inlineStr">
         <is>
-          <t>modellingAndValidation/LCIMethodAndAllocation</t>
+          <t>processDataSet/modellingAndValidation/LCIMethodAndAllocation</t>
         </is>
       </c>
     </row>
@@ -13230,12 +13230,12 @@
       <c r="AA135" t="inlineStr"/>
       <c r="AB135" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC135" t="inlineStr">
         <is>
-          <t>modellingAndValidation/LCIMethodAndAllocation/typeOfDataSet</t>
+          <t>processDataSet/modellingAndValidation/LCIMethodAndAllocation/typeOfDataSet</t>
         </is>
       </c>
     </row>
@@ -13355,12 +13355,12 @@
       <c r="AA136" t="inlineStr"/>
       <c r="AB136" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC136" t="inlineStr">
         <is>
-          <t>modellingAndValidation/LCIMethodAndAllocation/referenceToLCAMethodDetails</t>
+          <t>processDataSet/modellingAndValidation/LCIMethodAndAllocation/referenceToLCAMethodDetails</t>
         </is>
       </c>
     </row>
@@ -13461,12 +13461,12 @@
       <c r="AA137" t="inlineStr"/>
       <c r="AB137" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC137" t="inlineStr">
         <is>
-          <t>modellingAndValidation/LCIMethodAndAllocation/other</t>
+          <t>processDataSet/modellingAndValidation/LCIMethodAndAllocation/other</t>
         </is>
       </c>
     </row>
@@ -13576,12 +13576,12 @@
       <c r="AA138" t="inlineStr"/>
       <c r="AB138" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="AC138" t="inlineStr">
         <is>
-          <t>modellingAndValidation/LCIMethodAndAllocation/other/epd:subType</t>
+          <t>processDataSet/modellingAndValidation/LCIMethodAndAllocation/other/epd:subType</t>
         </is>
       </c>
     </row>
@@ -13659,12 +13659,12 @@
       <c r="AA139" t="inlineStr"/>
       <c r="AB139" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="AC139" t="inlineStr">
         <is>
-          <t>modellingAndValidation/LCIMethodAndAllocation/epd24:pcrCompliance</t>
+          <t>processDataSet/modellingAndValidation/LCIMethodAndAllocation/other/epd24:pcrCompliance</t>
         </is>
       </c>
     </row>
@@ -13750,12 +13750,12 @@
       <c r="AA140" t="inlineStr"/>
       <c r="AB140" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="AC140" t="inlineStr">
         <is>
-          <t>modellingAndValidation/LCIMethodAndAllocation/@epd24:allocation</t>
+          <t>processDataSet/modellingAndValidation/LCIMethodAndAllocation/other/epd24:pcrCompliance/@epd24:allocation</t>
         </is>
       </c>
     </row>
@@ -13846,12 +13846,12 @@
       <c r="AA141" t="inlineStr"/>
       <c r="AB141" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="AC141" t="inlineStr">
         <is>
-          <t>modellingAndValidation/LCIMethodAndAllocation/@epd24:cutOffRules</t>
+          <t>processDataSet/modellingAndValidation/LCIMethodAndAllocation/other/epd24:pcrCompliance/@epd24:cutOffRules</t>
         </is>
       </c>
     </row>
@@ -13943,12 +13943,12 @@
       <c r="AA142" t="inlineStr"/>
       <c r="AB142" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="AC142" t="inlineStr">
         <is>
-          <t>modellingAndValidation/LCIMethodAndAllocation/@epd24:upstreamDataDeviatingFromAllocationPrinciples</t>
+          <t>processDataSet/modellingAndValidation/LCIMethodAndAllocation/other/epd24:pcrCompliance/@epd24:upstreamDataDeviatingFromAllocationPrinciples</t>
         </is>
       </c>
     </row>
@@ -14051,12 +14051,12 @@
       <c r="AA143" t="inlineStr"/>
       <c r="AB143" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="AC143" t="inlineStr">
         <is>
-          <t>modellingAndValidation/LCIMethodAndAllocation/epd24:variability</t>
+          <t>processDataSet/modellingAndValidation/LCIMethodAndAllocation/other/epd24:variability</t>
         </is>
       </c>
     </row>
@@ -14142,12 +14142,12 @@
       <c r="AA144" t="inlineStr"/>
       <c r="AB144" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="AC144" t="inlineStr">
         <is>
-          <t>modellingAndValidation/LCIMethodAndAllocation/epd24:manufacturerVariability</t>
+          <t>processDataSet/modellingAndValidation/LCIMethodAndAllocation/other/epd24:variability/epd24:manufacturerVariability</t>
         </is>
       </c>
     </row>
@@ -14235,12 +14235,12 @@
       <c r="AA145" t="inlineStr"/>
       <c r="AB145" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>6</t>
         </is>
       </c>
       <c r="AC145" t="inlineStr">
         <is>
-          <t>modellingAndValidation/LCIMethodAndAllocation/@epd24:type</t>
+          <t>processDataSet/modellingAndValidation/LCIMethodAndAllocation/other/epd24:variability/epd24:manufacturerVariability/@epd24:type</t>
         </is>
       </c>
     </row>
@@ -14326,12 +14326,12 @@
       <c r="AA146" t="inlineStr"/>
       <c r="AB146" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>6</t>
         </is>
       </c>
       <c r="AC146" t="inlineStr">
         <is>
-          <t>modellingAndValidation/LCIMethodAndAllocation/@epd24:variation</t>
+          <t>processDataSet/modellingAndValidation/LCIMethodAndAllocation/other/epd24:variability/epd24:manufacturerVariability/@epd24:variation</t>
         </is>
       </c>
     </row>
@@ -14422,12 +14422,12 @@
       <c r="AA147" t="inlineStr"/>
       <c r="AB147" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>6</t>
         </is>
       </c>
       <c r="AC147" t="inlineStr">
         <is>
-          <t>modellingAndValidation/LCIMethodAndAllocation/@epd24:variationRange</t>
+          <t>processDataSet/modellingAndValidation/LCIMethodAndAllocation/other/epd24:variability/epd24:manufacturerVariability/@epd24:variationRange</t>
         </is>
       </c>
     </row>
@@ -14513,12 +14513,12 @@
       <c r="AA148" t="inlineStr"/>
       <c r="AB148" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="AC148" t="inlineStr">
         <is>
-          <t>modellingAndValidation/LCIMethodAndAllocation/epd24:productVariability</t>
+          <t>processDataSet/modellingAndValidation/LCIMethodAndAllocation/other/epd24:variability/epd24:productVariability</t>
         </is>
       </c>
     </row>
@@ -14605,12 +14605,12 @@
       <c r="AA149" t="inlineStr"/>
       <c r="AB149" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>6</t>
         </is>
       </c>
       <c r="AC149" t="inlineStr">
         <is>
-          <t>modellingAndValidation/LCIMethodAndAllocation/@epd24:type</t>
+          <t>processDataSet/modellingAndValidation/LCIMethodAndAllocation/other/epd24:variability/epd24:productVariability/@epd24:type</t>
         </is>
       </c>
     </row>
@@ -14696,12 +14696,12 @@
       <c r="AA150" t="inlineStr"/>
       <c r="AB150" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>6</t>
         </is>
       </c>
       <c r="AC150" t="inlineStr">
         <is>
-          <t>modellingAndValidation/LCIMethodAndAllocation/@epd24:variation</t>
+          <t>processDataSet/modellingAndValidation/LCIMethodAndAllocation/other/epd24:variability/epd24:productVariability/@epd24:variation</t>
         </is>
       </c>
     </row>
@@ -14792,12 +14792,12 @@
       <c r="AA151" t="inlineStr"/>
       <c r="AB151" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>6</t>
         </is>
       </c>
       <c r="AC151" t="inlineStr">
         <is>
-          <t>modellingAndValidation/LCIMethodAndAllocation/@epd24:variationRange</t>
+          <t>processDataSet/modellingAndValidation/LCIMethodAndAllocation/other/epd24:variability/epd24:productVariability/@epd24:variationRange</t>
         </is>
       </c>
     </row>
@@ -14883,12 +14883,12 @@
       <c r="AA152" t="inlineStr"/>
       <c r="AB152" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="AC152" t="inlineStr">
         <is>
-          <t>modellingAndValidation/LCIMethodAndAllocation/epd24:variabilityDescription</t>
+          <t>processDataSet/modellingAndValidation/LCIMethodAndAllocation/other/epd24:variability/epd24:variabilityDescription</t>
         </is>
       </c>
     </row>
@@ -14970,12 +14970,12 @@
       <c r="AA153" t="inlineStr"/>
       <c r="AB153" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AC153" t="inlineStr">
         <is>
-          <t>modellingAndValidation/dataSourcesTreatmentAndRepresentativeness</t>
+          <t>processDataSet/modellingAndValidation/dataSourcesTreatmentAndRepresentativeness</t>
         </is>
       </c>
     </row>
@@ -15077,12 +15077,12 @@
       <c r="AA154" t="inlineStr"/>
       <c r="AB154" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC154" t="inlineStr">
         <is>
-          <t>modellingAndValidation/dataSourcesTreatmentAndRepresentativeness/referenceToDataHandlingPrinciples</t>
+          <t>processDataSet/modellingAndValidation/dataSourcesTreatmentAndRepresentativeness/referenceToDataHandlingPrinciples</t>
         </is>
       </c>
     </row>
@@ -15202,12 +15202,12 @@
       <c r="AA155" t="inlineStr"/>
       <c r="AB155" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC155" t="inlineStr">
         <is>
-          <t>modellingAndValidation/dataSourcesTreatmentAndRepresentativeness/referenceToDataSource</t>
+          <t>processDataSet/modellingAndValidation/dataSourcesTreatmentAndRepresentativeness/referenceToDataSource</t>
         </is>
       </c>
     </row>
@@ -15327,12 +15327,12 @@
       <c r="AA156" t="inlineStr"/>
       <c r="AB156" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC156" t="inlineStr">
         <is>
-          <t>modellingAndValidation/dataSourcesTreatmentAndRepresentativeness/useAdviceForDataSet</t>
+          <t>processDataSet/modellingAndValidation/dataSourcesTreatmentAndRepresentativeness/useAdviceForDataSet</t>
         </is>
       </c>
     </row>
@@ -15418,12 +15418,12 @@
       <c r="AA157" t="inlineStr"/>
       <c r="AB157" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC157" t="inlineStr">
         <is>
-          <t>modellingAndValidation/dataSourcesTreatmentAndRepresentativeness/other</t>
+          <t>processDataSet/modellingAndValidation/dataSourcesTreatmentAndRepresentativeness/other</t>
         </is>
       </c>
     </row>
@@ -15517,12 +15517,12 @@
       <c r="AA158" t="inlineStr"/>
       <c r="AB158" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="AC158" t="inlineStr">
         <is>
-          <t>modellingAndValidation/dataSourcesTreatmentAndRepresentativeness/epd2:referenceToOriginalEPD</t>
+          <t>processDataSet/modellingAndValidation/dataSourcesTreatmentAndRepresentativeness/other/epd2:referenceToOriginalEPD</t>
         </is>
       </c>
     </row>
@@ -15614,12 +15614,12 @@
       <c r="AA159" t="inlineStr"/>
       <c r="AB159" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="AC159" t="inlineStr">
         <is>
-          <t>modellingAndValidation/epd24:manufacturers</t>
+          <t>processDataSet/modellingAndValidation/dataSourcesTreatmentAndRepresentativeness/other/epd24:manufacturers</t>
         </is>
       </c>
     </row>
@@ -15713,12 +15713,12 @@
       <c r="AA160" t="inlineStr"/>
       <c r="AB160" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="AC160" t="inlineStr">
         <is>
-          <t>modellingAndValidation/epd24:manufacturers/epd24:manufacturer</t>
+          <t>processDataSet/modellingAndValidation/dataSourcesTreatmentAndRepresentativeness/other/epd24:manufacturers/epd24:manufacturer</t>
         </is>
       </c>
     </row>
@@ -15816,12 +15816,12 @@
       <c r="AA161" t="inlineStr"/>
       <c r="AB161" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>6</t>
         </is>
       </c>
       <c r="AC161" t="inlineStr">
         <is>
-          <t>modellingAndValidation/epd24:manufacturers/epd24:contact</t>
+          <t>processDataSet/modellingAndValidation/dataSourcesTreatmentAndRepresentativeness/other/epd24:manufacturers/epd24:manufacturer/epd24:contact</t>
         </is>
       </c>
     </row>
@@ -15917,12 +15917,12 @@
       <c r="AA162" t="inlineStr"/>
       <c r="AB162" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>6</t>
         </is>
       </c>
       <c r="AC162" t="inlineStr">
         <is>
-          <t>modellingAndValidation/epd24:manufacturers/epd24:sites</t>
+          <t>processDataSet/modellingAndValidation/dataSourcesTreatmentAndRepresentativeness/other/epd24:manufacturers/epd24:manufacturer/epd24:sites</t>
         </is>
       </c>
     </row>
@@ -16016,12 +16016,12 @@
       <c r="AA163" t="inlineStr"/>
       <c r="AB163" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>7</t>
         </is>
       </c>
       <c r="AC163" t="inlineStr">
         <is>
-          <t>modellingAndValidation/epd24:manufacturers/epd24:site</t>
+          <t>processDataSet/modellingAndValidation/dataSourcesTreatmentAndRepresentativeness/other/epd24:manufacturers/epd24:manufacturer/epd24:sites/epd24:site</t>
         </is>
       </c>
     </row>
@@ -16119,12 +16119,12 @@
       <c r="AA164" t="inlineStr"/>
       <c r="AB164" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>8</t>
         </is>
       </c>
       <c r="AC164" t="inlineStr">
         <is>
-          <t>modellingAndValidation/epd24:manufacturers/epd24:name</t>
+          <t>processDataSet/modellingAndValidation/dataSourcesTreatmentAndRepresentativeness/other/epd24:manufacturers/epd24:manufacturer/epd24:sites/epd24:site/epd24:name</t>
         </is>
       </c>
     </row>
@@ -16222,12 +16222,12 @@
       <c r="AA165" t="inlineStr"/>
       <c r="AB165" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>8</t>
         </is>
       </c>
       <c r="AC165" t="inlineStr">
         <is>
-          <t>modellingAndValidation/epd24:manufacturers/epd24:facilityIdentifier</t>
+          <t>processDataSet/modellingAndValidation/dataSourcesTreatmentAndRepresentativeness/other/epd24:manufacturers/epd24:manufacturer/epd24:sites/epd24:site/epd24:facilityIdentifier</t>
         </is>
       </c>
     </row>
@@ -16325,12 +16325,12 @@
       <c r="AA166" t="inlineStr"/>
       <c r="AB166" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>8</t>
         </is>
       </c>
       <c r="AC166" t="inlineStr">
         <is>
-          <t>modellingAndValidation/epd24:manufacturers/epd24:olc</t>
+          <t>processDataSet/modellingAndValidation/dataSourcesTreatmentAndRepresentativeness/other/epd24:manufacturers/epd24:manufacturer/epd24:sites/epd24:site/epd24:olc</t>
         </is>
       </c>
     </row>
@@ -16428,12 +16428,12 @@
       <c r="AA167" t="inlineStr"/>
       <c r="AB167" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>8</t>
         </is>
       </c>
       <c r="AC167" t="inlineStr">
         <is>
-          <t>modellingAndValidation/epd24:manufacturers/epd24:geoCode</t>
+          <t>processDataSet/modellingAndValidation/dataSourcesTreatmentAndRepresentativeness/other/epd24:manufacturers/epd24:manufacturer/epd24:sites/epd24:site/epd24:geoCode</t>
         </is>
       </c>
     </row>
@@ -16531,12 +16531,12 @@
       <c r="AA168" t="inlineStr"/>
       <c r="AB168" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>8</t>
         </is>
       </c>
       <c r="AC168" t="inlineStr">
         <is>
-          <t>modellingAndValidation/epd24:manufacturers/epd24:streetAddress</t>
+          <t>processDataSet/modellingAndValidation/dataSourcesTreatmentAndRepresentativeness/other/epd24:manufacturers/epd24:manufacturer/epd24:sites/epd24:site/epd24:streetAddress</t>
         </is>
       </c>
     </row>
@@ -16630,12 +16630,12 @@
       <c r="AA169" t="inlineStr"/>
       <c r="AB169" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AC169" t="inlineStr">
         <is>
-          <t>modellingAndValidation/validation</t>
+          <t>processDataSet/modellingAndValidation/validation</t>
         </is>
       </c>
     </row>
@@ -16725,12 +16725,12 @@
       <c r="AA170" t="inlineStr"/>
       <c r="AB170" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC170" t="inlineStr">
         <is>
-          <t>modellingAndValidation/validation/review</t>
+          <t>processDataSet/modellingAndValidation/validation/review</t>
         </is>
       </c>
     </row>
@@ -16867,12 +16867,12 @@
       <c r="AA171" t="inlineStr"/>
       <c r="AB171" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="AC171" t="inlineStr">
         <is>
-          <t>modellingAndValidation/validation/@type</t>
+          <t>processDataSet/modellingAndValidation/validation/review/@type</t>
         </is>
       </c>
     </row>
@@ -16974,12 +16974,12 @@
       <c r="AA172" t="inlineStr"/>
       <c r="AB172" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="AC172" t="inlineStr">
         <is>
-          <t>modellingAndValidation/validation/reviewDetails</t>
+          <t>processDataSet/modellingAndValidation/validation/review/reviewDetails</t>
         </is>
       </c>
     </row>
@@ -17100,12 +17100,12 @@
       <c r="AA173" t="inlineStr"/>
       <c r="AB173" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="AC173" t="inlineStr">
         <is>
-          <t>modellingAndValidation/validation/referenceToNameOfReviewerAndInstitution</t>
+          <t>processDataSet/modellingAndValidation/validation/review/referenceToNameOfReviewerAndInstitution</t>
         </is>
       </c>
     </row>
@@ -17199,12 +17199,12 @@
       <c r="AA174" t="inlineStr"/>
       <c r="AB174" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="AC174" t="inlineStr">
         <is>
-          <t>modellingAndValidation/validation/referenceToCompleteReviewReport</t>
+          <t>processDataSet/modellingAndValidation/validation/review/referenceToCompleteReviewReport</t>
         </is>
       </c>
     </row>
@@ -17290,12 +17290,12 @@
       <c r="AA175" t="inlineStr"/>
       <c r="AB175" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC175" t="inlineStr">
         <is>
-          <t>modellingAndValidation/validation/other</t>
+          <t>processDataSet/modellingAndValidation/validation/other</t>
         </is>
       </c>
     </row>
@@ -17381,12 +17381,12 @@
       <c r="AA176" t="inlineStr"/>
       <c r="AB176" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AC176" t="inlineStr">
         <is>
-          <t>modellingAndValidation/complianceDeclarations</t>
+          <t>processDataSet/modellingAndValidation/complianceDeclarations</t>
         </is>
       </c>
     </row>
@@ -17476,12 +17476,12 @@
       <c r="AA177" t="inlineStr"/>
       <c r="AB177" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC177" t="inlineStr">
         <is>
-          <t>modellingAndValidation/complianceDeclarations/compliance</t>
+          <t>processDataSet/modellingAndValidation/complianceDeclarations/compliance</t>
         </is>
       </c>
     </row>
@@ -17600,12 +17600,12 @@
       <c r="AA178" t="inlineStr"/>
       <c r="AB178" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="AC178" t="inlineStr">
         <is>
-          <t>modellingAndValidation/complianceDeclarations/referenceToComplianceSystem</t>
+          <t>processDataSet/modellingAndValidation/complianceDeclarations/compliance/referenceToComplianceSystem</t>
         </is>
       </c>
     </row>
@@ -17691,12 +17691,12 @@
       <c r="AA179" t="inlineStr"/>
       <c r="AB179" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC179" t="inlineStr">
         <is>
-          <t>modellingAndValidation/complianceDeclarations/other</t>
+          <t>processDataSet/modellingAndValidation/complianceDeclarations/other</t>
         </is>
       </c>
     </row>
@@ -17787,7 +17787,7 @@
       </c>
       <c r="AC180" t="inlineStr">
         <is>
-          <t>modellingAndValidation/administrativeInformation</t>
+          <t>processDataSet/administrativeInformation</t>
         </is>
       </c>
     </row>
@@ -17869,12 +17869,12 @@
       <c r="AA181" t="inlineStr"/>
       <c r="AB181" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AC181" t="inlineStr">
         <is>
-          <t>modellingAndValidation/commissionerAndGoal</t>
+          <t>processDataSet/administrativeInformation/commissionerAndGoal</t>
         </is>
       </c>
     </row>
@@ -17984,12 +17984,12 @@
       <c r="AA182" t="inlineStr"/>
       <c r="AB182" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC182" t="inlineStr">
         <is>
-          <t>modellingAndValidation/commissionerAndGoal/referenceToCommissioner</t>
+          <t>processDataSet/administrativeInformation/commissionerAndGoal/referenceToCommissioner</t>
         </is>
       </c>
     </row>
@@ -18096,12 +18096,12 @@
       <c r="AA183" t="inlineStr"/>
       <c r="AB183" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC183" t="inlineStr">
         <is>
-          <t>modellingAndValidation/commissionerAndGoal/project</t>
+          <t>processDataSet/administrativeInformation/commissionerAndGoal/project</t>
         </is>
       </c>
     </row>
@@ -18195,12 +18195,12 @@
       <c r="AA184" t="inlineStr"/>
       <c r="AB184" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC184" t="inlineStr">
         <is>
-          <t>modellingAndValidation/commissionerAndGoal/intendedApplications</t>
+          <t>processDataSet/administrativeInformation/commissionerAndGoal/intendedApplications</t>
         </is>
       </c>
     </row>
@@ -18286,12 +18286,12 @@
       <c r="AA185" t="inlineStr"/>
       <c r="AB185" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC185" t="inlineStr">
         <is>
-          <t>modellingAndValidation/commissionerAndGoal/other</t>
+          <t>processDataSet/administrativeInformation/commissionerAndGoal/other</t>
         </is>
       </c>
     </row>
@@ -18373,12 +18373,12 @@
       <c r="AA186" t="inlineStr"/>
       <c r="AB186" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AC186" t="inlineStr">
         <is>
-          <t>modellingAndValidation/dataGenerator</t>
+          <t>processDataSet/administrativeInformation/dataGenerator</t>
         </is>
       </c>
     </row>
@@ -18480,12 +18480,12 @@
       <c r="AA187" t="inlineStr"/>
       <c r="AB187" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC187" t="inlineStr">
         <is>
-          <t>modellingAndValidation/dataGenerator/referenceToPersonOrEntityGeneratingTheDataSet</t>
+          <t>processDataSet/administrativeInformation/dataGenerator/referenceToPersonOrEntityGeneratingTheDataSet</t>
         </is>
       </c>
     </row>
@@ -18571,12 +18571,12 @@
       <c r="AA188" t="inlineStr"/>
       <c r="AB188" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC188" t="inlineStr">
         <is>
-          <t>modellingAndValidation/dataGenerator/other</t>
+          <t>processDataSet/administrativeInformation/dataGenerator/other</t>
         </is>
       </c>
     </row>
@@ -18662,12 +18662,12 @@
       <c r="AA189" t="inlineStr"/>
       <c r="AB189" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AC189" t="inlineStr">
         <is>
-          <t>modellingAndValidation/dataEntryBy</t>
+          <t>processDataSet/administrativeInformation/dataEntryBy</t>
         </is>
       </c>
     </row>
@@ -18766,12 +18766,12 @@
       <c r="AA190" t="inlineStr"/>
       <c r="AB190" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC190" t="inlineStr">
         <is>
-          <t>modellingAndValidation/dataEntryBy/timeStamp</t>
+          <t>processDataSet/administrativeInformation/dataEntryBy/timeStamp</t>
         </is>
       </c>
     </row>
@@ -18874,12 +18874,12 @@
       <c r="AA191" t="inlineStr"/>
       <c r="AB191" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC191" t="inlineStr">
         <is>
-          <t>modellingAndValidation/dataEntryBy/referenceToDataSetFormat</t>
+          <t>processDataSet/administrativeInformation/dataEntryBy/referenceToDataSetFormat</t>
         </is>
       </c>
     </row>
@@ -18965,12 +18965,12 @@
       <c r="AA192" t="inlineStr"/>
       <c r="AB192" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC192" t="inlineStr">
         <is>
-          <t>modellingAndValidation/dataEntryBy/other</t>
+          <t>processDataSet/administrativeInformation/dataEntryBy/other</t>
         </is>
       </c>
     </row>
@@ -19056,12 +19056,12 @@
       <c r="AA193" t="inlineStr"/>
       <c r="AB193" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AC193" t="inlineStr">
         <is>
-          <t>modellingAndValidation/publicationAndOwnership</t>
+          <t>processDataSet/administrativeInformation/publicationAndOwnership</t>
         </is>
       </c>
     </row>
@@ -19163,12 +19163,12 @@
       <c r="AA194" t="inlineStr"/>
       <c r="AB194" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC194" t="inlineStr">
         <is>
-          <t>modellingAndValidation/publicationAndOwnership/dataSetVersion</t>
+          <t>processDataSet/administrativeInformation/publicationAndOwnership/dataSetVersion</t>
         </is>
       </c>
     </row>
@@ -19263,12 +19263,12 @@
       <c r="AA195" t="inlineStr"/>
       <c r="AB195" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC195" t="inlineStr">
         <is>
-          <t>modellingAndValidation/publicationAndOwnership/referenceToPrecedingDataSetVersion</t>
+          <t>processDataSet/administrativeInformation/publicationAndOwnership/referenceToPrecedingDataSetVersion</t>
         </is>
       </c>
     </row>
@@ -19358,12 +19358,12 @@
       <c r="AA196" t="inlineStr"/>
       <c r="AB196" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC196" t="inlineStr">
         <is>
-          <t>modellingAndValidation/publicationAndOwnership/permanentDataSetURI</t>
+          <t>processDataSet/administrativeInformation/publicationAndOwnership/permanentDataSetURI</t>
         </is>
       </c>
     </row>
@@ -19461,12 +19461,12 @@
       <c r="AA197" t="inlineStr"/>
       <c r="AB197" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC197" t="inlineStr">
         <is>
-          <t>modellingAndValidation/publicationAndOwnership/dateOfLastRevision</t>
+          <t>processDataSet/administrativeInformation/publicationAndOwnership/dateOfLastRevision</t>
         </is>
       </c>
     </row>
@@ -19576,12 +19576,12 @@
       <c r="AA198" t="inlineStr"/>
       <c r="AB198" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC198" t="inlineStr">
         <is>
-          <t>modellingAndValidation/publicationAndOwnership/referenceToRegistrationAuthority</t>
+          <t>processDataSet/administrativeInformation/publicationAndOwnership/referenceToRegistrationAuthority</t>
         </is>
       </c>
     </row>
@@ -19692,12 +19692,12 @@
       <c r="AA199" t="inlineStr"/>
       <c r="AB199" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC199" t="inlineStr">
         <is>
-          <t>modellingAndValidation/publicationAndOwnership/registrationNumber</t>
+          <t>processDataSet/administrativeInformation/publicationAndOwnership/registrationNumber</t>
         </is>
       </c>
     </row>
@@ -19799,12 +19799,12 @@
       <c r="AA200" t="inlineStr"/>
       <c r="AB200" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC200" t="inlineStr">
         <is>
-          <t>modellingAndValidation/publicationAndOwnership/referenceToOwnershipOfDataSet</t>
+          <t>processDataSet/administrativeInformation/publicationAndOwnership/referenceToOwnershipOfDataSet</t>
         </is>
       </c>
     </row>
@@ -19906,12 +19906,12 @@
       <c r="AA201" t="inlineStr"/>
       <c r="AB201" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC201" t="inlineStr">
         <is>
-          <t>modellingAndValidation/publicationAndOwnership/copyright</t>
+          <t>processDataSet/administrativeInformation/publicationAndOwnership/copyright</t>
         </is>
       </c>
     </row>
@@ -20014,12 +20014,12 @@
       <c r="AA202" t="inlineStr"/>
       <c r="AB202" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC202" t="inlineStr">
         <is>
-          <t>modellingAndValidation/publicationAndOwnership/licenseType</t>
+          <t>processDataSet/administrativeInformation/publicationAndOwnership/licenseType</t>
         </is>
       </c>
     </row>
@@ -20113,12 +20113,12 @@
       <c r="AA203" t="inlineStr"/>
       <c r="AB203" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC203" t="inlineStr">
         <is>
-          <t>modellingAndValidation/publicationAndOwnership/accessRestrictions</t>
+          <t>processDataSet/administrativeInformation/publicationAndOwnership/accessRestrictions</t>
         </is>
       </c>
     </row>
@@ -20204,12 +20204,12 @@
       <c r="AA204" t="inlineStr"/>
       <c r="AB204" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC204" t="inlineStr">
         <is>
-          <t>modellingAndValidation/publicationAndOwnership/other</t>
+          <t>processDataSet/administrativeInformation/publicationAndOwnership/other</t>
         </is>
       </c>
     </row>
@@ -20315,12 +20315,12 @@
       <c r="AA205" t="inlineStr"/>
       <c r="AB205" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="AC205" t="inlineStr">
         <is>
-          <t>modellingAndValidation/publicationAndOwnership/other/referenceToPublisher</t>
+          <t>processDataSet/administrativeInformation/publicationAndOwnership/other/referenceToPublisher</t>
         </is>
       </c>
     </row>
@@ -20410,12 +20410,12 @@
       <c r="AA206" t="inlineStr"/>
       <c r="AB206" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AC206" t="inlineStr">
         <is>
-          <t>exchanges</t>
+          <t>processDataSet/exchanges</t>
         </is>
       </c>
     </row>
@@ -20501,12 +20501,12 @@
       <c r="AA207" t="inlineStr"/>
       <c r="AB207" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AC207" t="inlineStr">
         <is>
-          <t>exchanges/exchange</t>
+          <t>processDataSet/exchanges/exchange</t>
         </is>
       </c>
     </row>
@@ -20596,12 +20596,12 @@
       <c r="AA208" t="inlineStr"/>
       <c r="AB208" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC208" t="inlineStr">
         <is>
-          <t>exchanges/exchange/@dataSetInternalID</t>
+          <t>processDataSet/exchanges/exchange/@dataSetInternalID</t>
         </is>
       </c>
     </row>
@@ -20695,12 +20695,12 @@
       <c r="AA209" t="inlineStr"/>
       <c r="AB209" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC209" t="inlineStr">
         <is>
-          <t>exchanges/exchange/referenceToFlowDataSet</t>
+          <t>processDataSet/exchanges/exchange/referenceToFlowDataSet</t>
         </is>
       </c>
     </row>
@@ -20787,12 +20787,12 @@
       <c r="AA210" t="inlineStr"/>
       <c r="AB210" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC210" t="inlineStr">
         <is>
-          <t>exchanges/exchange/functionType</t>
+          <t>processDataSet/exchanges/exchange/functionType</t>
         </is>
       </c>
     </row>
@@ -20888,12 +20888,12 @@
       <c r="AA211" t="inlineStr"/>
       <c r="AB211" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC211" t="inlineStr">
         <is>
-          <t>exchanges/exchange/exchangeDirection</t>
+          <t>processDataSet/exchanges/exchange/exchangeDirection</t>
         </is>
       </c>
     </row>
@@ -20987,12 +20987,12 @@
       <c r="AA212" t="inlineStr"/>
       <c r="AB212" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC212" t="inlineStr">
         <is>
-          <t>exchanges/exchange/meanAmount</t>
+          <t>processDataSet/exchanges/exchange/meanAmount</t>
         </is>
       </c>
     </row>
@@ -21086,12 +21086,12 @@
       <c r="AA213" t="inlineStr"/>
       <c r="AB213" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC213" t="inlineStr">
         <is>
-          <t>exchanges/exchange/generalComment</t>
+          <t>processDataSet/exchanges/exchange/generalComment</t>
         </is>
       </c>
     </row>
@@ -21177,12 +21177,12 @@
       <c r="AA214" t="inlineStr"/>
       <c r="AB214" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC214" t="inlineStr">
         <is>
-          <t>exchanges/exchange/other</t>
+          <t>processDataSet/exchanges/exchange/other</t>
         </is>
       </c>
     </row>
@@ -21272,12 +21272,12 @@
       <c r="AA215" t="inlineStr"/>
       <c r="AB215" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="AC215" t="inlineStr">
         <is>
-          <t>exchanges/exchange/epd:amount</t>
+          <t>processDataSet/exchanges/exchange/other/epd:amount</t>
         </is>
       </c>
     </row>
@@ -21379,12 +21379,12 @@
       <c r="AA216" t="inlineStr"/>
       <c r="AB216" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="AC216" t="inlineStr">
         <is>
-          <t>exchanges/exchange/@epd:module</t>
+          <t>processDataSet/exchanges/exchange/other/epd:amount/@epd:module</t>
         </is>
       </c>
     </row>
@@ -21470,12 +21470,12 @@
       <c r="AA217" t="inlineStr"/>
       <c r="AB217" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="AC217" t="inlineStr">
         <is>
-          <t>exchanges/exchange/@epd:scenario</t>
+          <t>processDataSet/exchanges/exchange/other/epd:amount/@epd:scenario</t>
         </is>
       </c>
     </row>
@@ -21569,12 +21569,12 @@
       <c r="AA218" t="inlineStr"/>
       <c r="AB218" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="AC218" t="inlineStr">
         <is>
-          <t>exchanges/exchange/epd:referenceToUnitGroupDataSet</t>
+          <t>processDataSet/exchanges/exchange/other/epd:referenceToUnitGroupDataSet</t>
         </is>
       </c>
     </row>
@@ -21660,12 +21660,12 @@
       <c r="AA219" t="inlineStr"/>
       <c r="AB219" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AC219" t="inlineStr">
         <is>
-          <t>LCIAResults</t>
+          <t>processDataSet/LCIAResults</t>
         </is>
       </c>
     </row>
@@ -21747,12 +21747,12 @@
       <c r="AA220" t="inlineStr"/>
       <c r="AB220" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AC220" t="inlineStr">
         <is>
-          <t>LCIAResults/LCIAResult</t>
+          <t>processDataSet/LCIAResults/LCIAResult</t>
         </is>
       </c>
     </row>
@@ -21846,12 +21846,12 @@
       <c r="AA221" t="inlineStr"/>
       <c r="AB221" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC221" t="inlineStr">
         <is>
-          <t>LCIAResults/LCIAResult/referenceToLCIAMethodDataSet</t>
+          <t>processDataSet/LCIAResults/LCIAResult/referenceToLCIAMethodDataSet</t>
         </is>
       </c>
     </row>
@@ -21945,12 +21945,12 @@
       <c r="AA222" t="inlineStr"/>
       <c r="AB222" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC222" t="inlineStr">
         <is>
-          <t>LCIAResults/LCIAResult/generalComment</t>
+          <t>processDataSet/LCIAResults/LCIAResult/generalComment</t>
         </is>
       </c>
     </row>
@@ -22036,12 +22036,12 @@
       <c r="AA223" t="inlineStr"/>
       <c r="AB223" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC223" t="inlineStr">
         <is>
-          <t>LCIAResults/LCIAResult/other</t>
+          <t>processDataSet/LCIAResults/LCIAResult/other</t>
         </is>
       </c>
     </row>
@@ -22131,12 +22131,12 @@
       <c r="AA224" t="inlineStr"/>
       <c r="AB224" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="AC224" t="inlineStr">
         <is>
-          <t>LCIAResults/LCIAResult/epd:amount</t>
+          <t>processDataSet/LCIAResults/LCIAResult/other/epd:amount</t>
         </is>
       </c>
     </row>
@@ -22242,12 +22242,12 @@
       <c r="AA225" t="inlineStr"/>
       <c r="AB225" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="AC225" t="inlineStr">
         <is>
-          <t>LCIAResults/LCIAResult/@epd:module</t>
+          <t>processDataSet/LCIAResults/LCIAResult/other/epd:amount/@epd:module</t>
         </is>
       </c>
     </row>
@@ -22333,12 +22333,12 @@
       <c r="AA226" t="inlineStr"/>
       <c r="AB226" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="AC226" t="inlineStr">
         <is>
-          <t>LCIAResults/LCIAResult/@epd:scenario</t>
+          <t>processDataSet/LCIAResults/LCIAResult/other/epd:amount/@epd:scenario</t>
         </is>
       </c>
     </row>
@@ -22444,12 +22444,12 @@
       <c r="AA227" t="inlineStr"/>
       <c r="AB227" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="AC227" t="inlineStr">
         <is>
-          <t>LCIAResults/LCIAResult/epd:referenceToUnitGroupDataSet</t>
+          <t>processDataSet/LCIAResults/LCIAResult/other/epd:referenceToUnitGroupDataSet</t>
         </is>
       </c>
     </row>

</xml_diff>